<commit_message>
final list and data xlsx
</commit_message>
<xml_diff>
--- a/list and data.xlsx
+++ b/list and data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13320" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13320" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pa2" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3137" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3640" uniqueCount="438">
   <si>
     <t>instrument</t>
   </si>
@@ -1234,6 +1234,114 @@
   </si>
   <si>
     <t>pbreq</t>
+  </si>
+  <si>
+    <t>house</t>
+  </si>
+  <si>
+    <t>'ADM'</t>
+  </si>
+  <si>
+    <t>'bpid'</t>
+  </si>
+  <si>
+    <t>'ADMU00000'</t>
+  </si>
+  <si>
+    <t>'Margin1'}</t>
+  </si>
+  <si>
+    <t>'BPS'</t>
+  </si>
+  <si>
+    <t>'BPSS00000'</t>
+  </si>
+  <si>
+    <t>'FCSU00000'</t>
+  </si>
+  <si>
+    <t>'OMFA00000'</t>
+  </si>
+  <si>
+    <t>'SFL'</t>
+  </si>
+  <si>
+    <t>'SFLU00000'</t>
+  </si>
+  <si>
+    <t>'stressl'</t>
+  </si>
+  <si>
+    <t>'acctype'</t>
+  </si>
+  <si>
+    <t>'deltanetexps'</t>
+  </si>
+  <si>
+    <t>'deltanetexpsconv'</t>
+  </si>
+  <si>
+    <t>'rcconv'</t>
+  </si>
+  <si>
+    <t>'marginconv'</t>
+  </si>
+  <si>
+    <t>'slconv'</t>
+  </si>
+  <si>
+    <t>25303.7488275}</t>
+  </si>
+  <si>
+    <t>'Client'</t>
+  </si>
+  <si>
+    <t>3945.0289125}</t>
+  </si>
+  <si>
+    <t>24196.17733}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">this is </t>
+  </si>
+  <si>
+    <t>calculated</t>
+  </si>
+  <si>
+    <t>accounts</t>
+  </si>
+  <si>
+    <t>a/c</t>
+  </si>
+  <si>
+    <t>final</t>
+  </si>
+  <si>
+    <t>'OMFRule'</t>
+  </si>
+  <si>
+    <t>'Rule'</t>
+  </si>
+  <si>
+    <t>'OMFFinal'</t>
+  </si>
+  <si>
+    <t>'Final'</t>
+  </si>
+  <si>
+    <t>'FCSRule'</t>
+  </si>
+  <si>
+    <t>'FCSFinal'</t>
+  </si>
+  <si>
+    <t>'stresslconv'</t>
+  </si>
+  <si>
+    <t>'OMFA00000'}</t>
+  </si>
+  <si>
+    <t>'FCSU00000'}</t>
   </si>
 </sst>
 </file>
@@ -2850,6 +2958,194 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Straight Arrow Connector 16"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="48358425" y="5257800"/>
+          <a:ext cx="6096000" cy="2314576"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="63500">
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>79</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Arrow Connector 17"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="48968025" y="4686300"/>
+          <a:ext cx="5486400" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="63500">
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="19" name="Straight Arrow Connector 18"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="50187225" y="3533775"/>
+          <a:ext cx="4267200" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="63500">
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>81</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>88</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="22" name="Straight Arrow Connector 21"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="50272950" y="1476375"/>
+          <a:ext cx="4181475" cy="2828925"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="63500">
+          <a:tailEnd type="triangle" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3118,8 +3414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC86"/>
   <sheetViews>
-    <sheetView topLeftCell="R10" workbookViewId="0">
-      <selection activeCell="AK73" sqref="AK73"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7612,10 +7908,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE54"/>
+  <dimension ref="A1:AE61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10186,6 +10482,114 @@
       </c>
       <c r="J54" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>324</v>
+      </c>
+      <c r="B57" t="s">
+        <v>403</v>
+      </c>
+      <c r="C57" t="s">
+        <v>404</v>
+      </c>
+      <c r="D57" t="s">
+        <v>405</v>
+      </c>
+      <c r="E57" t="s">
+        <v>326</v>
+      </c>
+      <c r="F57" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>324</v>
+      </c>
+      <c r="B58" t="s">
+        <v>407</v>
+      </c>
+      <c r="C58" t="s">
+        <v>404</v>
+      </c>
+      <c r="D58" t="s">
+        <v>408</v>
+      </c>
+      <c r="E58" t="s">
+        <v>326</v>
+      </c>
+      <c r="F58" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>324</v>
+      </c>
+      <c r="B59" t="s">
+        <v>325</v>
+      </c>
+      <c r="C59" t="s">
+        <v>404</v>
+      </c>
+      <c r="D59" t="s">
+        <v>409</v>
+      </c>
+      <c r="E59" t="s">
+        <v>326</v>
+      </c>
+      <c r="F59" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>324</v>
+      </c>
+      <c r="B60" t="s">
+        <v>332</v>
+      </c>
+      <c r="C60" t="s">
+        <v>404</v>
+      </c>
+      <c r="D60" t="s">
+        <v>410</v>
+      </c>
+      <c r="E60" t="s">
+        <v>326</v>
+      </c>
+      <c r="F60" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>324</v>
+      </c>
+      <c r="B61" t="s">
+        <v>411</v>
+      </c>
+      <c r="C61" t="s">
+        <v>404</v>
+      </c>
+      <c r="D61" t="s">
+        <v>412</v>
+      </c>
+      <c r="E61" t="s">
+        <v>326</v>
+      </c>
+      <c r="F61" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -10287,10 +10691,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CA48"/>
+  <dimension ref="A1:EM52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="DD4" workbookViewId="0">
+      <selection activeCell="DU22" sqref="DU22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10305,9 +10709,10 @@
     <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="7.140625" customWidth="1"/>
     <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>293</v>
       </c>
@@ -10315,7 +10720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -10344,7 +10749,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>294</v>
       </c>
@@ -10378,7 +10783,7 @@
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -10413,7 +10818,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -10448,7 +10853,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>294</v>
       </c>
@@ -10483,7 +10888,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>311</v>
       </c>
@@ -10511,8 +10916,16 @@
       <c r="AI7" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="BX7" s="3" t="str">
+        <f>cons!A56</f>
+        <v>house</v>
+      </c>
+      <c r="BY7" s="3" t="str">
+        <f>cons!B56</f>
+        <v>list</v>
+      </c>
+    </row>
+    <row r="8" spans="1:81" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>294</v>
       </c>
@@ -10537,8 +10950,32 @@
       <c r="R8" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="BX8" s="5" t="str">
+        <f>cons!A57</f>
+        <v>{'bp'</v>
+      </c>
+      <c r="BY8" s="5" t="str">
+        <f>cons!B57</f>
+        <v>'ADM'</v>
+      </c>
+      <c r="BZ8" s="5" t="str">
+        <f>cons!C57</f>
+        <v>'bpid'</v>
+      </c>
+      <c r="CA8" s="5" t="str">
+        <f>cons!D57</f>
+        <v>'ADMU00000'</v>
+      </c>
+      <c r="CB8" s="5" t="str">
+        <f>cons!E57</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC8" s="5" t="str">
+        <f>cons!F57</f>
+        <v>'Margin1'}</v>
+      </c>
+    </row>
+    <row r="9" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>294</v>
       </c>
@@ -10563,8 +11000,32 @@
       <c r="R9" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="BX9" s="5" t="str">
+        <f>cons!A58</f>
+        <v>{'bp'</v>
+      </c>
+      <c r="BY9" s="5" t="str">
+        <f>cons!B58</f>
+        <v>'BPS'</v>
+      </c>
+      <c r="BZ9" s="5" t="str">
+        <f>cons!C58</f>
+        <v>'bpid'</v>
+      </c>
+      <c r="CA9" s="5" t="str">
+        <f>cons!D58</f>
+        <v>'BPSS00000'</v>
+      </c>
+      <c r="CB9" s="5" t="str">
+        <f>cons!E58</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC9" s="5" t="str">
+        <f>cons!F58</f>
+        <v>'Margin1'}</v>
+      </c>
+    </row>
+    <row r="10" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>294</v>
       </c>
@@ -10589,8 +11050,32 @@
       <c r="R10" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="BX10" s="5" t="str">
+        <f>cons!A59</f>
+        <v>{'bp'</v>
+      </c>
+      <c r="BY10" s="5" t="str">
+        <f>cons!B59</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="BZ10" s="5" t="str">
+        <f>cons!C59</f>
+        <v>'bpid'</v>
+      </c>
+      <c r="CA10" s="5" t="str">
+        <f>cons!D59</f>
+        <v>'FCSU00000'</v>
+      </c>
+      <c r="CB10" s="5" t="str">
+        <f>cons!E59</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC10" s="5" t="str">
+        <f>cons!F59</f>
+        <v>'Margin1'}</v>
+      </c>
+    </row>
+    <row r="11" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>294</v>
       </c>
@@ -10615,8 +11100,32 @@
       <c r="R11" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="BX11" s="5" t="str">
+        <f>cons!A60</f>
+        <v>{'bp'</v>
+      </c>
+      <c r="BY11" s="5" t="str">
+        <f>cons!B60</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="BZ11" s="5" t="str">
+        <f>cons!C60</f>
+        <v>'bpid'</v>
+      </c>
+      <c r="CA11" s="5" t="str">
+        <f>cons!D60</f>
+        <v>'OMFA00000'</v>
+      </c>
+      <c r="CB11" s="5" t="str">
+        <f>cons!E60</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC11" s="5" t="str">
+        <f>cons!F60</f>
+        <v>'Margin1'}</v>
+      </c>
+    </row>
+    <row r="12" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>294</v>
       </c>
@@ -10638,8 +11147,32 @@
       <c r="G12" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="BX12" s="5" t="str">
+        <f>cons!A61</f>
+        <v>{'bp'</v>
+      </c>
+      <c r="BY12" s="5" t="str">
+        <f>cons!B61</f>
+        <v>'SFL'</v>
+      </c>
+      <c r="BZ12" s="5" t="str">
+        <f>cons!C61</f>
+        <v>'bpid'</v>
+      </c>
+      <c r="CA12" s="5" t="str">
+        <f>cons!D61</f>
+        <v>'SFLU00000'</v>
+      </c>
+      <c r="CB12" s="5" t="str">
+        <f>cons!E61</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC12" s="5" t="str">
+        <f>cons!F61</f>
+        <v>'Margin1'}</v>
+      </c>
+    </row>
+    <row r="13" spans="1:81" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>311</v>
       </c>
@@ -10668,7 +11201,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>316</v>
       </c>
@@ -10682,7 +11215,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>316</v>
       </c>
@@ -10696,7 +11229,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>316</v>
       </c>
@@ -10710,7 +11243,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="17" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>316</v>
       </c>
@@ -10723,8 +11256,12 @@
       <c r="S17" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="18" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="BX17" s="3" t="str">
+        <f>'pa2'!A50</f>
+        <v>currency</v>
+      </c>
+    </row>
+    <row r="18" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>316</v>
       </c>
@@ -10737,8 +11274,32 @@
       <c r="S18" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="19" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="BX18" s="5" t="str">
+        <f>'pa2'!A51</f>
+        <v>{'curra'</v>
+      </c>
+      <c r="BY18" s="5" t="str">
+        <f>'pa2'!B51</f>
+        <v>'USD',</v>
+      </c>
+      <c r="BZ18" s="5" t="str">
+        <f>'pa2'!C51</f>
+        <v>'currb'</v>
+      </c>
+      <c r="CA18" s="5" t="str">
+        <f>'pa2'!D51</f>
+        <v>'NZD',</v>
+      </c>
+      <c r="CB18" s="5" t="str">
+        <f>'pa2'!E51</f>
+        <v>'rate'</v>
+      </c>
+      <c r="CC18" s="5" t="str">
+        <f>'pa2'!F51</f>
+        <v>1.481701}</v>
+      </c>
+    </row>
+    <row r="19" spans="1:143" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>316</v>
       </c>
@@ -10752,7 +11313,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="20" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>316</v>
       </c>
@@ -10760,7 +11321,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="21" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>316</v>
       </c>
@@ -10783,7 +11344,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="22" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>316</v>
       </c>
@@ -10802,8 +11363,14 @@
       <c r="X22" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CZ22" t="s">
+        <v>424</v>
+      </c>
+      <c r="DB22" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="23" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>316</v>
       </c>
@@ -10822,8 +11389,14 @@
       <c r="X23" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CZ23" t="s">
+        <v>425</v>
+      </c>
+      <c r="DB23" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="24" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U24" t="s">
         <v>316</v>
       </c>
@@ -10872,8 +11445,42 @@
       <c r="CA24" s="3" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="25" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK24" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="CL24" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="CM24" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="CN24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="DL24" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="DM24" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="DN24" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="DO24" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="DP24" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="DQ24" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="DR24" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="DS24" s="3"/>
+    </row>
+    <row r="25" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U25" t="s">
         <v>316</v>
       </c>
@@ -10904,8 +11511,170 @@
       <c r="BV25" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="26" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK25" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL25" t="s">
+        <v>338</v>
+      </c>
+      <c r="CM25" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN25" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO25" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP25">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="CQ25" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR25">
+        <v>-65320</v>
+      </c>
+      <c r="CS25" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT25">
+        <v>17077.5</v>
+      </c>
+      <c r="CU25" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV25">
+        <v>2662.5</v>
+      </c>
+      <c r="CW25" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX25" t="s">
+        <v>353</v>
+      </c>
+      <c r="CY25" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ25">
+        <v>-58614.093999999997</v>
+      </c>
+      <c r="DA25" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB25">
+        <v>14415</v>
+      </c>
+      <c r="DC25" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD25">
+        <v>-86848.561693893993</v>
+      </c>
+      <c r="DE25" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF25">
+        <v>21358.7199149999</v>
+      </c>
+      <c r="DG25" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH25">
+        <v>3945.0289124999999</v>
+      </c>
+      <c r="DI25" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ25" t="s">
+        <v>420</v>
+      </c>
+      <c r="DL25" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM25" t="s">
+        <v>341</v>
+      </c>
+      <c r="DN25" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO25" t="s">
+        <v>368</v>
+      </c>
+      <c r="DP25" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ25">
+        <v>0</v>
+      </c>
+      <c r="DR25" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS25">
+        <v>0</v>
+      </c>
+      <c r="DT25" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU25">
+        <v>0</v>
+      </c>
+      <c r="DV25" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW25">
+        <v>0</v>
+      </c>
+      <c r="DX25" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY25" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ25" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA25">
+        <v>0</v>
+      </c>
+      <c r="EB25" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC25">
+        <v>0</v>
+      </c>
+      <c r="ED25" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE25">
+        <v>0</v>
+      </c>
+      <c r="EF25" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG25">
+        <v>0</v>
+      </c>
+      <c r="EH25" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI25">
+        <v>0</v>
+      </c>
+      <c r="EJ25" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK25">
+        <v>0</v>
+      </c>
+      <c r="EL25" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM25" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="26" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U26" t="s">
         <v>316</v>
       </c>
@@ -10936,8 +11705,170 @@
       <c r="BV26" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="27" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK26" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL26" t="s">
+        <v>338</v>
+      </c>
+      <c r="CM26" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN26" t="s">
+        <v>381</v>
+      </c>
+      <c r="CO26" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP26">
+        <v>0</v>
+      </c>
+      <c r="CQ26" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR26">
+        <v>0</v>
+      </c>
+      <c r="CS26" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT26">
+        <v>0</v>
+      </c>
+      <c r="CU26" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV26">
+        <v>0</v>
+      </c>
+      <c r="CW26" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX26" t="s">
+        <v>353</v>
+      </c>
+      <c r="CY26" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ26">
+        <v>0</v>
+      </c>
+      <c r="DA26" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB26">
+        <v>0</v>
+      </c>
+      <c r="DC26" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD26">
+        <v>0</v>
+      </c>
+      <c r="DE26" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF26">
+        <v>0</v>
+      </c>
+      <c r="DG26" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH26">
+        <v>0</v>
+      </c>
+      <c r="DI26" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ26" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL26" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM26" t="s">
+        <v>341</v>
+      </c>
+      <c r="DN26" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO26" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP26" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ26">
+        <v>0</v>
+      </c>
+      <c r="DR26" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS26">
+        <v>-741600</v>
+      </c>
+      <c r="DT26" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU26">
+        <v>1305280</v>
+      </c>
+      <c r="DV26" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW26">
+        <v>1305280</v>
+      </c>
+      <c r="DX26" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY26" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ26" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA26">
+        <v>-741600</v>
+      </c>
+      <c r="EB26" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC26">
+        <v>0</v>
+      </c>
+      <c r="ED26" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE26">
+        <v>-741600</v>
+      </c>
+      <c r="EF26" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG26">
+        <v>0</v>
+      </c>
+      <c r="EH26" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI26">
+        <v>1305280</v>
+      </c>
+      <c r="EJ26" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK26">
+        <v>1305280</v>
+      </c>
+      <c r="EL26" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM26" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="27" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U27" t="s">
         <v>316</v>
       </c>
@@ -10968,8 +11899,170 @@
       <c r="BV27" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="28" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK27" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL27" t="s">
+        <v>340</v>
+      </c>
+      <c r="CM27" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN27" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO27" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP27">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="CQ27" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR27">
+        <v>0</v>
+      </c>
+      <c r="CS27" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT27">
+        <v>2662.5</v>
+      </c>
+      <c r="CU27" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV27">
+        <v>2662.5</v>
+      </c>
+      <c r="CW27" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX27" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY27" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ27">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="DA27" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB27">
+        <v>0</v>
+      </c>
+      <c r="DC27" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD27">
+        <v>9936.1476261059997</v>
+      </c>
+      <c r="DE27" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF27">
+        <v>0</v>
+      </c>
+      <c r="DG27" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH27">
+        <v>3945.0289124999999</v>
+      </c>
+      <c r="DI27" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ27" t="s">
+        <v>422</v>
+      </c>
+      <c r="DL27" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM27" t="s">
+        <v>338</v>
+      </c>
+      <c r="DN27" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO27" t="s">
+        <v>368</v>
+      </c>
+      <c r="DP27" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ27">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="DR27" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS27">
+        <v>0</v>
+      </c>
+      <c r="DT27" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU27">
+        <v>2662.5</v>
+      </c>
+      <c r="DV27" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW27">
+        <v>17077.5</v>
+      </c>
+      <c r="DX27" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY27" t="s">
+        <v>353</v>
+      </c>
+      <c r="DZ27" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA27">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="EB27" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC27">
+        <v>0</v>
+      </c>
+      <c r="ED27" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE27">
+        <v>9936.1476261059997</v>
+      </c>
+      <c r="EF27" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG27">
+        <v>0</v>
+      </c>
+      <c r="EH27" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI27">
+        <v>25303.7488275</v>
+      </c>
+      <c r="EJ27" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK27">
+        <v>3945.0289124999999</v>
+      </c>
+      <c r="EL27" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM27" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="28" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U28" t="s">
         <v>316</v>
       </c>
@@ -11000,8 +12093,170 @@
       <c r="BV28" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="29" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK28" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL28" t="s">
+        <v>340</v>
+      </c>
+      <c r="CM28" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN28" t="s">
+        <v>381</v>
+      </c>
+      <c r="CO28" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP28">
+        <v>0</v>
+      </c>
+      <c r="CQ28" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR28">
+        <v>0</v>
+      </c>
+      <c r="CS28" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT28">
+        <v>0</v>
+      </c>
+      <c r="CU28" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV28">
+        <v>0</v>
+      </c>
+      <c r="CW28" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX28" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY28" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ28">
+        <v>0</v>
+      </c>
+      <c r="DA28" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB28">
+        <v>0</v>
+      </c>
+      <c r="DC28" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD28">
+        <v>0</v>
+      </c>
+      <c r="DE28" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF28">
+        <v>0</v>
+      </c>
+      <c r="DG28" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH28">
+        <v>0</v>
+      </c>
+      <c r="DI28" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ28" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL28" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM28" t="s">
+        <v>338</v>
+      </c>
+      <c r="DN28" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO28" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP28" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ28">
+        <v>0</v>
+      </c>
+      <c r="DR28" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS28">
+        <v>0</v>
+      </c>
+      <c r="DT28" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU28">
+        <v>0</v>
+      </c>
+      <c r="DV28" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW28">
+        <v>0</v>
+      </c>
+      <c r="DX28" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY28" t="s">
+        <v>353</v>
+      </c>
+      <c r="DZ28" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA28">
+        <v>0</v>
+      </c>
+      <c r="EB28" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC28">
+        <v>0</v>
+      </c>
+      <c r="ED28" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE28">
+        <v>0</v>
+      </c>
+      <c r="EF28" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG28">
+        <v>0</v>
+      </c>
+      <c r="EH28" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI28">
+        <v>0</v>
+      </c>
+      <c r="EJ28" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK28">
+        <v>0</v>
+      </c>
+      <c r="EL28" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM28" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="29" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U29" t="s">
         <v>316</v>
       </c>
@@ -11032,8 +12287,170 @@
       <c r="BV29" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="30" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK29" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL29" t="s">
+        <v>337</v>
+      </c>
+      <c r="CM29" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN29" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO29" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP29">
+        <v>1948.175</v>
+      </c>
+      <c r="CQ29" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR29">
+        <v>0</v>
+      </c>
+      <c r="CS29" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT29">
+        <v>0</v>
+      </c>
+      <c r="CU29" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV29">
+        <v>0</v>
+      </c>
+      <c r="CW29" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX29" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY29" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ29">
+        <v>1948.175</v>
+      </c>
+      <c r="DA29" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB29">
+        <v>0</v>
+      </c>
+      <c r="DC29" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD29">
+        <v>2886.6128456749998</v>
+      </c>
+      <c r="DE29" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF29">
+        <v>0</v>
+      </c>
+      <c r="DG29" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH29">
+        <v>0</v>
+      </c>
+      <c r="DI29" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ29" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL29" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM29" t="s">
+        <v>342</v>
+      </c>
+      <c r="DN29" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO29" t="s">
+        <v>368</v>
+      </c>
+      <c r="DP29" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ29">
+        <v>1948.175</v>
+      </c>
+      <c r="DR29" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS29">
+        <v>0</v>
+      </c>
+      <c r="DT29" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU29">
+        <v>0</v>
+      </c>
+      <c r="DV29" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW29">
+        <v>0</v>
+      </c>
+      <c r="DX29" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY29" t="s">
+        <v>353</v>
+      </c>
+      <c r="DZ29" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA29">
+        <v>1948.175</v>
+      </c>
+      <c r="EB29" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC29">
+        <v>0</v>
+      </c>
+      <c r="ED29" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE29">
+        <v>2886.6128456749998</v>
+      </c>
+      <c r="EF29" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG29">
+        <v>0</v>
+      </c>
+      <c r="EH29" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI29">
+        <v>0</v>
+      </c>
+      <c r="EJ29" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK29">
+        <v>0</v>
+      </c>
+      <c r="EL29" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM29" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="30" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U30" t="s">
         <v>316</v>
       </c>
@@ -11064,8 +12481,170 @@
       <c r="BV30" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="31" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK30" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL30" t="s">
+        <v>337</v>
+      </c>
+      <c r="CM30" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN30" t="s">
+        <v>381</v>
+      </c>
+      <c r="CO30" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP30">
+        <v>0</v>
+      </c>
+      <c r="CQ30" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR30">
+        <v>-1854000</v>
+      </c>
+      <c r="CS30" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT30">
+        <v>407597</v>
+      </c>
+      <c r="CU30" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV30">
+        <v>407597</v>
+      </c>
+      <c r="CW30" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX30" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY30" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ30">
+        <v>-1854000</v>
+      </c>
+      <c r="DA30" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB30">
+        <v>0</v>
+      </c>
+      <c r="DC30" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD30">
+        <v>-1854000</v>
+      </c>
+      <c r="DE30" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF30">
+        <v>0</v>
+      </c>
+      <c r="DG30" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH30">
+        <v>407597</v>
+      </c>
+      <c r="DI30" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ30" t="s">
+        <v>391</v>
+      </c>
+      <c r="DL30" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM30" t="s">
+        <v>342</v>
+      </c>
+      <c r="DN30" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO30" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP30" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ30">
+        <v>0</v>
+      </c>
+      <c r="DR30" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS30">
+        <v>0</v>
+      </c>
+      <c r="DT30" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU30">
+        <v>0</v>
+      </c>
+      <c r="DV30" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW30">
+        <v>0</v>
+      </c>
+      <c r="DX30" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY30" t="s">
+        <v>353</v>
+      </c>
+      <c r="DZ30" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA30">
+        <v>0</v>
+      </c>
+      <c r="EB30" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC30">
+        <v>0</v>
+      </c>
+      <c r="ED30" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE30">
+        <v>0</v>
+      </c>
+      <c r="EF30" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG30">
+        <v>0</v>
+      </c>
+      <c r="EH30" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI30">
+        <v>0</v>
+      </c>
+      <c r="EJ30" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK30">
+        <v>0</v>
+      </c>
+      <c r="EL30" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM30" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="31" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U31" t="s">
         <v>316</v>
       </c>
@@ -11096,8 +12675,143 @@
       <c r="BV31" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="32" spans="1:79" x14ac:dyDescent="0.25">
+      <c r="CK31" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL31" t="s">
+        <v>341</v>
+      </c>
+      <c r="CM31" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN31" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO31" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP31">
+        <v>0</v>
+      </c>
+      <c r="CQ31" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR31">
+        <v>0</v>
+      </c>
+      <c r="CS31" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT31">
+        <v>0</v>
+      </c>
+      <c r="CU31" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV31">
+        <v>0</v>
+      </c>
+      <c r="CW31" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX31" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY31" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ31">
+        <v>0</v>
+      </c>
+      <c r="DA31" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB31">
+        <v>0</v>
+      </c>
+      <c r="DC31" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD31">
+        <v>0</v>
+      </c>
+      <c r="DE31" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF31">
+        <v>0</v>
+      </c>
+      <c r="DG31" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH31">
+        <v>0</v>
+      </c>
+      <c r="DI31" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ31" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL31" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM31" t="s">
+        <v>339</v>
+      </c>
+      <c r="DN31" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO31" t="s">
+        <v>368</v>
+      </c>
+      <c r="DP31" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ31">
+        <v>0</v>
+      </c>
+      <c r="DR31" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS31">
+        <v>-65320</v>
+      </c>
+      <c r="DT31" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU31">
+        <v>16330</v>
+      </c>
+      <c r="DV31" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW31">
+        <v>16330</v>
+      </c>
+      <c r="DX31" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY31" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ31" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA31">
+        <v>-65320</v>
+      </c>
+      <c r="EB31" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC31">
+        <v>0</v>
+      </c>
+      <c r="ED31" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="32" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U32" t="s">
         <v>316</v>
       </c>
@@ -11128,8 +12842,113 @@
       <c r="BV32" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="33" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="CK32" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL32" t="s">
+        <v>341</v>
+      </c>
+      <c r="CM32" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN32" t="s">
+        <v>381</v>
+      </c>
+      <c r="CO32" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP32">
+        <v>0</v>
+      </c>
+      <c r="CQ32" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR32">
+        <v>-741600</v>
+      </c>
+      <c r="CS32" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT32">
+        <v>1305280</v>
+      </c>
+      <c r="CU32" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV32">
+        <v>1305280</v>
+      </c>
+      <c r="CW32" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX32" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY32" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ32">
+        <v>-741600</v>
+      </c>
+      <c r="DA32" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB32">
+        <v>0</v>
+      </c>
+      <c r="DC32" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD32">
+        <v>-741600</v>
+      </c>
+      <c r="DE32" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF32">
+        <v>0</v>
+      </c>
+      <c r="DG32" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH32">
+        <v>1305280</v>
+      </c>
+      <c r="DI32" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ32" t="s">
+        <v>393</v>
+      </c>
+      <c r="DL32">
+        <v>-96784.709319999994</v>
+      </c>
+      <c r="DM32" t="s">
+        <v>417</v>
+      </c>
+      <c r="DN32">
+        <v>0</v>
+      </c>
+      <c r="DO32" t="s">
+        <v>418</v>
+      </c>
+      <c r="DP32">
+        <v>24196.177329999999</v>
+      </c>
+      <c r="DQ32" t="s">
+        <v>435</v>
+      </c>
+      <c r="DR32">
+        <v>24196.177329999999</v>
+      </c>
+      <c r="DS32" t="s">
+        <v>404</v>
+      </c>
+      <c r="DT32" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="33" spans="1:143" x14ac:dyDescent="0.25">
       <c r="U33" t="s">
         <v>316</v>
       </c>
@@ -11160,8 +12979,170 @@
       <c r="BV33" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="34" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="CK33" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL33" t="s">
+        <v>342</v>
+      </c>
+      <c r="CM33" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN33" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO33" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP33">
+        <v>1948.175</v>
+      </c>
+      <c r="CQ33" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR33">
+        <v>0</v>
+      </c>
+      <c r="CS33" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT33">
+        <v>0</v>
+      </c>
+      <c r="CU33" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV33">
+        <v>0</v>
+      </c>
+      <c r="CW33" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX33" t="s">
+        <v>353</v>
+      </c>
+      <c r="CY33" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ33">
+        <v>1948.175</v>
+      </c>
+      <c r="DA33" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB33">
+        <v>0</v>
+      </c>
+      <c r="DC33" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD33">
+        <v>2886.6128456749998</v>
+      </c>
+      <c r="DE33" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF33">
+        <v>0</v>
+      </c>
+      <c r="DG33" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH33">
+        <v>0</v>
+      </c>
+      <c r="DI33" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ33" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL33" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM33" t="s">
+        <v>339</v>
+      </c>
+      <c r="DN33" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO33" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP33" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ33">
+        <v>0</v>
+      </c>
+      <c r="DR33" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS33">
+        <v>0</v>
+      </c>
+      <c r="DT33" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU33">
+        <v>0</v>
+      </c>
+      <c r="DV33" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW33">
+        <v>0</v>
+      </c>
+      <c r="DX33" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY33" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ33" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA33">
+        <v>0</v>
+      </c>
+      <c r="EB33" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC33">
+        <v>0</v>
+      </c>
+      <c r="ED33" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE33">
+        <v>0</v>
+      </c>
+      <c r="EF33" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG33">
+        <v>0</v>
+      </c>
+      <c r="EH33" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI33">
+        <v>0</v>
+      </c>
+      <c r="EJ33" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK33">
+        <v>0</v>
+      </c>
+      <c r="EL33" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM33" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="34" spans="1:143" x14ac:dyDescent="0.25">
       <c r="AA34" s="3" t="s">
         <v>1</v>
       </c>
@@ -11195,8 +13176,170 @@
       <c r="BV34" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="35" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="CK34" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL34" t="s">
+        <v>342</v>
+      </c>
+      <c r="CM34" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN34" t="s">
+        <v>381</v>
+      </c>
+      <c r="CO34" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP34">
+        <v>0</v>
+      </c>
+      <c r="CQ34" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR34">
+        <v>0</v>
+      </c>
+      <c r="CS34" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT34">
+        <v>0</v>
+      </c>
+      <c r="CU34" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV34">
+        <v>0</v>
+      </c>
+      <c r="CW34" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX34" t="s">
+        <v>353</v>
+      </c>
+      <c r="CY34" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ34">
+        <v>0</v>
+      </c>
+      <c r="DA34" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB34">
+        <v>0</v>
+      </c>
+      <c r="DC34" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD34">
+        <v>0</v>
+      </c>
+      <c r="DE34" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF34">
+        <v>0</v>
+      </c>
+      <c r="DG34" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH34">
+        <v>0</v>
+      </c>
+      <c r="DI34" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ34" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL34" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM34" t="s">
+        <v>337</v>
+      </c>
+      <c r="DN34" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO34" t="s">
+        <v>368</v>
+      </c>
+      <c r="DP34" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ34">
+        <v>1948.175</v>
+      </c>
+      <c r="DR34" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS34">
+        <v>0</v>
+      </c>
+      <c r="DT34" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU34">
+        <v>0</v>
+      </c>
+      <c r="DV34" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW34">
+        <v>0</v>
+      </c>
+      <c r="DX34" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY34" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ34" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA34">
+        <v>1948.175</v>
+      </c>
+      <c r="EB34" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC34">
+        <v>0</v>
+      </c>
+      <c r="ED34" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE34">
+        <v>2886.6128456749998</v>
+      </c>
+      <c r="EF34" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG34">
+        <v>0</v>
+      </c>
+      <c r="EH34" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI34">
+        <v>0</v>
+      </c>
+      <c r="EJ34" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK34">
+        <v>0</v>
+      </c>
+      <c r="EL34" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM34" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="35" spans="1:143" x14ac:dyDescent="0.25">
       <c r="AA35" t="s">
         <v>324</v>
       </c>
@@ -11263,8 +13406,170 @@
       <c r="BV35" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="36" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="CK35" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL35" t="s">
+        <v>339</v>
+      </c>
+      <c r="CM35" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN35" t="s">
+        <v>368</v>
+      </c>
+      <c r="CO35" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP35">
+        <v>0</v>
+      </c>
+      <c r="CQ35" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR35">
+        <v>-65320</v>
+      </c>
+      <c r="CS35" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT35">
+        <v>16330</v>
+      </c>
+      <c r="CU35" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV35">
+        <v>16330</v>
+      </c>
+      <c r="CW35" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX35" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY35" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ35">
+        <v>-65320</v>
+      </c>
+      <c r="DA35" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB35">
+        <v>0</v>
+      </c>
+      <c r="DC35" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD35">
+        <v>-96784.709319999994</v>
+      </c>
+      <c r="DE35" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF35">
+        <v>0</v>
+      </c>
+      <c r="DG35" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH35">
+        <v>24196.177329999999</v>
+      </c>
+      <c r="DI35" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ35" t="s">
+        <v>423</v>
+      </c>
+      <c r="DL35" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM35" t="s">
+        <v>337</v>
+      </c>
+      <c r="DN35" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO35" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP35" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ35">
+        <v>0</v>
+      </c>
+      <c r="DR35" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS35">
+        <v>-1854000</v>
+      </c>
+      <c r="DT35" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU35">
+        <v>407597</v>
+      </c>
+      <c r="DV35" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW35">
+        <v>407597</v>
+      </c>
+      <c r="DX35" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY35" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ35" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA35">
+        <v>-1854000</v>
+      </c>
+      <c r="EB35" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC35">
+        <v>0</v>
+      </c>
+      <c r="ED35" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE35">
+        <v>-1854000</v>
+      </c>
+      <c r="EF35" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG35">
+        <v>0</v>
+      </c>
+      <c r="EH35" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI35">
+        <v>407597</v>
+      </c>
+      <c r="EJ35" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK35">
+        <v>407597</v>
+      </c>
+      <c r="EL35" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM35" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="36" spans="1:143" x14ac:dyDescent="0.25">
       <c r="AA36" t="s">
         <v>324</v>
       </c>
@@ -11331,8 +13636,170 @@
       <c r="BV36" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="37" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="CK36" t="s">
+        <v>316</v>
+      </c>
+      <c r="CL36" t="s">
+        <v>339</v>
+      </c>
+      <c r="CM36" t="s">
+        <v>26</v>
+      </c>
+      <c r="CN36" t="s">
+        <v>381</v>
+      </c>
+      <c r="CO36" t="s">
+        <v>379</v>
+      </c>
+      <c r="CP36">
+        <v>0</v>
+      </c>
+      <c r="CQ36" t="s">
+        <v>395</v>
+      </c>
+      <c r="CR36">
+        <v>0</v>
+      </c>
+      <c r="CS36" t="s">
+        <v>413</v>
+      </c>
+      <c r="CT36">
+        <v>0</v>
+      </c>
+      <c r="CU36" t="s">
+        <v>386</v>
+      </c>
+      <c r="CV36">
+        <v>0</v>
+      </c>
+      <c r="CW36" t="s">
+        <v>414</v>
+      </c>
+      <c r="CX36" t="s">
+        <v>421</v>
+      </c>
+      <c r="CY36" t="s">
+        <v>415</v>
+      </c>
+      <c r="CZ36">
+        <v>0</v>
+      </c>
+      <c r="DA36" t="s">
+        <v>400</v>
+      </c>
+      <c r="DB36">
+        <v>0</v>
+      </c>
+      <c r="DC36" t="s">
+        <v>416</v>
+      </c>
+      <c r="DD36">
+        <v>0</v>
+      </c>
+      <c r="DE36" t="s">
+        <v>417</v>
+      </c>
+      <c r="DF36">
+        <v>0</v>
+      </c>
+      <c r="DG36" t="s">
+        <v>418</v>
+      </c>
+      <c r="DH36">
+        <v>0</v>
+      </c>
+      <c r="DI36" t="s">
+        <v>419</v>
+      </c>
+      <c r="DJ36" t="s">
+        <v>243</v>
+      </c>
+      <c r="DL36" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM36" t="s">
+        <v>340</v>
+      </c>
+      <c r="DN36" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO36" t="s">
+        <v>368</v>
+      </c>
+      <c r="DP36" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ36">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="DR36" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS36">
+        <v>0</v>
+      </c>
+      <c r="DT36" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU36">
+        <v>2662.5</v>
+      </c>
+      <c r="DV36" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW36">
+        <v>2662.5</v>
+      </c>
+      <c r="DX36" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY36" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ36" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA36">
+        <v>6705.9059999999999</v>
+      </c>
+      <c r="EB36" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC36">
+        <v>0</v>
+      </c>
+      <c r="ED36" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE36">
+        <v>9936.1476261059997</v>
+      </c>
+      <c r="EF36" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG36">
+        <v>0</v>
+      </c>
+      <c r="EH36" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI36">
+        <v>3945.0289124999999</v>
+      </c>
+      <c r="EJ36" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK36">
+        <v>3945.0289124999999</v>
+      </c>
+      <c r="EL36" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM36" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="37" spans="1:143" x14ac:dyDescent="0.25">
       <c r="AA37" t="s">
         <v>324</v>
       </c>
@@ -11381,8 +13848,92 @@
       <c r="AP37" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="38" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="DL37" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM37" t="s">
+        <v>340</v>
+      </c>
+      <c r="DN37" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO37" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP37" t="s">
+        <v>379</v>
+      </c>
+      <c r="DQ37">
+        <v>0</v>
+      </c>
+      <c r="DR37" t="s">
+        <v>395</v>
+      </c>
+      <c r="DS37">
+        <v>0</v>
+      </c>
+      <c r="DT37" t="s">
+        <v>413</v>
+      </c>
+      <c r="DU37">
+        <v>0</v>
+      </c>
+      <c r="DV37" t="s">
+        <v>386</v>
+      </c>
+      <c r="DW37">
+        <v>0</v>
+      </c>
+      <c r="DX37" t="s">
+        <v>414</v>
+      </c>
+      <c r="DY37" t="s">
+        <v>421</v>
+      </c>
+      <c r="DZ37" t="s">
+        <v>415</v>
+      </c>
+      <c r="EA37">
+        <v>0</v>
+      </c>
+      <c r="EB37" t="s">
+        <v>400</v>
+      </c>
+      <c r="EC37">
+        <v>0</v>
+      </c>
+      <c r="ED37" t="s">
+        <v>416</v>
+      </c>
+      <c r="EE37">
+        <v>0</v>
+      </c>
+      <c r="EF37" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG37">
+        <v>0</v>
+      </c>
+      <c r="EH37" t="s">
+        <v>418</v>
+      </c>
+      <c r="EI37">
+        <v>0</v>
+      </c>
+      <c r="EJ37" t="s">
+        <v>435</v>
+      </c>
+      <c r="EK37">
+        <v>0</v>
+      </c>
+      <c r="EL37" t="s">
+        <v>404</v>
+      </c>
+      <c r="EM37" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="38" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -11440,8 +13991,38 @@
       <c r="AP38" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="39" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="DL38" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM38" t="s">
+        <v>429</v>
+      </c>
+      <c r="DN38" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO38" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP38" t="s">
+        <v>414</v>
+      </c>
+      <c r="DQ38" t="s">
+        <v>430</v>
+      </c>
+      <c r="DR38" t="s">
+        <v>417</v>
+      </c>
+      <c r="DS38">
+        <v>0</v>
+      </c>
+      <c r="DT38" t="s">
+        <v>404</v>
+      </c>
+      <c r="DU38" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="39" spans="1:143" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>324</v>
       </c>
@@ -11490,8 +14071,46 @@
       <c r="P39" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="40" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BX39" s="3" t="str">
+        <f>pbreq!L18</f>
+        <v>pbreq</v>
+      </c>
+      <c r="BY39" s="3" t="str">
+        <f>pbreq!M18</f>
+        <v>list</v>
+      </c>
+      <c r="DL39" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM39" t="s">
+        <v>431</v>
+      </c>
+      <c r="DN39" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO39" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP39" t="s">
+        <v>414</v>
+      </c>
+      <c r="DQ39" t="s">
+        <v>432</v>
+      </c>
+      <c r="DR39" t="s">
+        <v>417</v>
+      </c>
+      <c r="DS39">
+        <v>0</v>
+      </c>
+      <c r="DT39" t="s">
+        <v>404</v>
+      </c>
+      <c r="DU39" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="40" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>324</v>
       </c>
@@ -11540,8 +14159,166 @@
       <c r="P40" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="42" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BX40" s="5" t="str">
+        <f>pbreq!L19</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY40" s="5" t="str">
+        <f>pbreq!M19</f>
+        <v>'margin'</v>
+      </c>
+      <c r="BZ40" s="5" t="str">
+        <f>pbreq!N19</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA40" s="5" t="str">
+        <f>pbreq!O19</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="CB40" s="5" t="str">
+        <f>pbreq!P19</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC40" s="5" t="str">
+        <f>pbreq!Q19</f>
+        <v>'Margin2'</v>
+      </c>
+      <c r="CD40" s="5" t="str">
+        <f>pbreq!R19</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE40" s="5" t="str">
+        <f>pbreq!S19</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF40" s="5" t="str">
+        <f>pbreq!T19</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG40" s="5">
+        <f>pbreq!U19</f>
+        <v>16330</v>
+      </c>
+      <c r="CH40" s="5" t="str">
+        <f>pbreq!V19</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI40" s="5" t="str">
+        <f>pbreq!W19</f>
+        <v>-65320.0}</v>
+      </c>
+      <c r="DL40" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM40" t="s">
+        <v>433</v>
+      </c>
+      <c r="DN40" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO40" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP40" t="s">
+        <v>414</v>
+      </c>
+      <c r="DQ40" t="s">
+        <v>430</v>
+      </c>
+      <c r="DR40" t="s">
+        <v>417</v>
+      </c>
+      <c r="DS40">
+        <v>0</v>
+      </c>
+      <c r="DT40" t="s">
+        <v>404</v>
+      </c>
+      <c r="DU40" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="41" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BX41" s="5" t="str">
+        <f>pbreq!L20</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY41" s="5" t="str">
+        <f>pbreq!M20</f>
+        <v>'margin'</v>
+      </c>
+      <c r="BZ41" s="5" t="str">
+        <f>pbreq!N20</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA41" s="5" t="str">
+        <f>pbreq!O20</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="CB41" s="5" t="str">
+        <f>pbreq!P20</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC41" s="5" t="str">
+        <f>pbreq!Q20</f>
+        <v>'Margin4'</v>
+      </c>
+      <c r="CD41" s="5" t="str">
+        <f>pbreq!R20</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE41" s="5" t="str">
+        <f>pbreq!S20</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF41" s="5" t="str">
+        <f>pbreq!T20</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG41" s="5">
+        <f>pbreq!U20</f>
+        <v>2662.5</v>
+      </c>
+      <c r="CH41" s="5" t="str">
+        <f>pbreq!V20</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI41" s="5" t="str">
+        <f>pbreq!W20</f>
+        <v>0.0}</v>
+      </c>
+      <c r="DL41" t="s">
+        <v>316</v>
+      </c>
+      <c r="DM41" t="s">
+        <v>434</v>
+      </c>
+      <c r="DN41" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO41" t="s">
+        <v>381</v>
+      </c>
+      <c r="DP41" t="s">
+        <v>414</v>
+      </c>
+      <c r="DQ41" t="s">
+        <v>432</v>
+      </c>
+      <c r="DR41" t="s">
+        <v>417</v>
+      </c>
+      <c r="DS41">
+        <v>0</v>
+      </c>
+      <c r="DT41" t="s">
+        <v>404</v>
+      </c>
+      <c r="DU41" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="42" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AR42" s="3" t="s">
         <v>1</v>
       </c>
@@ -11563,8 +14340,56 @@
       <c r="AX42" s="3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="43" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BX42" s="5" t="str">
+        <f>pbreq!L21</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY42" s="5" t="str">
+        <f>pbreq!M21</f>
+        <v>'margin'</v>
+      </c>
+      <c r="BZ42" s="5" t="str">
+        <f>pbreq!N21</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA42" s="5" t="str">
+        <f>pbreq!O21</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="CB42" s="5" t="str">
+        <f>pbreq!P21</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC42" s="5" t="str">
+        <f>pbreq!Q21</f>
+        <v>'Sum'</v>
+      </c>
+      <c r="CD42" s="5" t="str">
+        <f>pbreq!R21</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE42" s="5" t="str">
+        <f>pbreq!S21</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF42" s="5" t="str">
+        <f>pbreq!T21</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG42" s="5">
+        <f>pbreq!U21</f>
+        <v>2662.5</v>
+      </c>
+      <c r="CH42" s="5" t="str">
+        <f>pbreq!V21</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI42" s="5" t="str">
+        <f>pbreq!W21</f>
+        <v>0.0}</v>
+      </c>
+    </row>
+    <row r="43" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AR43" t="s">
         <v>324</v>
       </c>
@@ -11637,8 +14462,56 @@
       <c r="BO43" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="44" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BX43" s="5" t="str">
+        <f>pbreq!L22</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY43" s="5" t="str">
+        <f>pbreq!M22</f>
+        <v>'margin'</v>
+      </c>
+      <c r="BZ43" s="5" t="str">
+        <f>pbreq!N22</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA43" s="5" t="str">
+        <f>pbreq!O22</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="CB43" s="5" t="str">
+        <f>pbreq!P22</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC43" s="5" t="str">
+        <f>pbreq!Q22</f>
+        <v>'Margin2'</v>
+      </c>
+      <c r="CD43" s="5" t="str">
+        <f>pbreq!R22</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE43" s="5" t="str">
+        <f>pbreq!S22</f>
+        <v>'NZD'</v>
+      </c>
+      <c r="CF43" s="5" t="str">
+        <f>pbreq!T22</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG43" s="5">
+        <f>pbreq!U22</f>
+        <v>407597</v>
+      </c>
+      <c r="CH43" s="5" t="str">
+        <f>pbreq!V22</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI43" s="5" t="str">
+        <f>pbreq!W22</f>
+        <v>-1854000.0}</v>
+      </c>
+    </row>
+    <row r="44" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O44" s="5" t="str">
         <f>'pa2'!N82</f>
         <v>option</v>
@@ -11791,8 +14664,56 @@
       <c r="BO44" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="45" spans="1:74" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="BX44" s="5" t="str">
+        <f>pbreq!L23</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY44" s="5" t="str">
+        <f>pbreq!M23</f>
+        <v>'margin'</v>
+      </c>
+      <c r="BZ44" s="5" t="str">
+        <f>pbreq!N23</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA44" s="5" t="str">
+        <f>pbreq!O23</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="CB44" s="5" t="str">
+        <f>pbreq!P23</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC44" s="5" t="str">
+        <f>pbreq!Q23</f>
+        <v>'Margin2'</v>
+      </c>
+      <c r="CD44" s="5" t="str">
+        <f>pbreq!R23</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE44" s="5" t="str">
+        <f>pbreq!S23</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF44" s="5" t="str">
+        <f>pbreq!T23</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG44" s="5">
+        <f>pbreq!U23</f>
+        <v>0</v>
+      </c>
+      <c r="CH44" s="5" t="str">
+        <f>pbreq!V23</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI44" s="5" t="str">
+        <f>pbreq!W23</f>
+        <v>0.0}</v>
+      </c>
+    </row>
+    <row r="45" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O45" t="str">
         <f>'pa2'!N83</f>
         <v>{'comm'</v>
@@ -11977,8 +14898,56 @@
       <c r="BO45" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="46" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BX45" s="5" t="str">
+        <f>pbreq!L24</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY45" s="5" t="str">
+        <f>pbreq!M24</f>
+        <v>'margin'</v>
+      </c>
+      <c r="BZ45" s="5" t="str">
+        <f>pbreq!N24</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA45" s="5" t="str">
+        <f>pbreq!O24</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="CB45" s="5" t="str">
+        <f>pbreq!P24</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC45" s="5" t="str">
+        <f>pbreq!Q24</f>
+        <v>'Margin3'</v>
+      </c>
+      <c r="CD45" s="5" t="str">
+        <f>pbreq!R24</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE45" s="5" t="str">
+        <f>pbreq!S24</f>
+        <v>'NZD'</v>
+      </c>
+      <c r="CF45" s="5" t="str">
+        <f>pbreq!T24</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG45" s="5">
+        <f>pbreq!U24</f>
+        <v>1305280</v>
+      </c>
+      <c r="CH45" s="5" t="str">
+        <f>pbreq!V24</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI45" s="5" t="str">
+        <f>pbreq!W24</f>
+        <v>-741600.0}</v>
+      </c>
+    </row>
+    <row r="46" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O46" t="str">
         <f>'pa2'!N84</f>
         <v>{'comm'</v>
@@ -12163,8 +15132,56 @@
       <c r="BO46" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="47" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BX46" s="5" t="str">
+        <f>pbreq!L25</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY46" s="5" t="str">
+        <f>pbreq!M25</f>
+        <v>'rc'</v>
+      </c>
+      <c r="BZ46" s="5" t="str">
+        <f>pbreq!N25</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA46" s="5" t="str">
+        <f>pbreq!O25</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="CB46" s="5" t="str">
+        <f>pbreq!P25</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC46" s="5" t="str">
+        <f>pbreq!Q25</f>
+        <v>'Margin2'</v>
+      </c>
+      <c r="CD46" s="5" t="str">
+        <f>pbreq!R25</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE46" s="5" t="str">
+        <f>pbreq!S25</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF46" s="5" t="str">
+        <f>pbreq!T25</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG46" s="5">
+        <f>pbreq!U25</f>
+        <v>16330</v>
+      </c>
+      <c r="CH46" s="5" t="str">
+        <f>pbreq!V25</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI46" s="5" t="str">
+        <f>pbreq!W25</f>
+        <v>-65320.0}</v>
+      </c>
+    </row>
+    <row r="47" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O47" t="str">
         <f>'pa2'!N85</f>
         <v>{'comm'</v>
@@ -12277,8 +15294,56 @@
         <f>'pa2'!AO85</f>
         <v>2615.0}</v>
       </c>
-    </row>
-    <row r="48" spans="1:74" x14ac:dyDescent="0.25">
+      <c r="BX47" s="5" t="str">
+        <f>pbreq!L26</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY47" s="5" t="str">
+        <f>pbreq!M26</f>
+        <v>'rc'</v>
+      </c>
+      <c r="BZ47" s="5" t="str">
+        <f>pbreq!N26</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA47" s="5" t="str">
+        <f>pbreq!O26</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="CB47" s="5" t="str">
+        <f>pbreq!P26</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC47" s="5" t="str">
+        <f>pbreq!Q26</f>
+        <v>'Margin4'</v>
+      </c>
+      <c r="CD47" s="5" t="str">
+        <f>pbreq!R26</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE47" s="5" t="str">
+        <f>pbreq!S26</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF47" s="5" t="str">
+        <f>pbreq!T26</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG47" s="5">
+        <f>pbreq!U26</f>
+        <v>2662.5</v>
+      </c>
+      <c r="CH47" s="5" t="str">
+        <f>pbreq!V26</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI47" s="5" t="str">
+        <f>pbreq!W26</f>
+        <v>0.0}</v>
+      </c>
+    </row>
+    <row r="48" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O48" t="str">
         <f>'pa2'!N86</f>
         <v>{'comm'</v>
@@ -12391,7 +15456,206 @@
         <f>'pa2'!AO86</f>
         <v>2615.0}</v>
       </c>
-    </row>
+      <c r="BX48" s="5" t="str">
+        <f>pbreq!L27</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY48" s="5" t="str">
+        <f>pbreq!M27</f>
+        <v>'rc'</v>
+      </c>
+      <c r="BZ48" s="5" t="str">
+        <f>pbreq!N27</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA48" s="5" t="str">
+        <f>pbreq!O27</f>
+        <v>'FCS'</v>
+      </c>
+      <c r="CB48" s="5" t="str">
+        <f>pbreq!P27</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC48" s="5" t="str">
+        <f>pbreq!Q27</f>
+        <v>'Sum'</v>
+      </c>
+      <c r="CD48" s="5" t="str">
+        <f>pbreq!R27</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE48" s="5" t="str">
+        <f>pbreq!S27</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF48" s="5" t="str">
+        <f>pbreq!T27</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG48" s="5">
+        <f>pbreq!U27</f>
+        <v>17077.5</v>
+      </c>
+      <c r="CH48" s="5" t="str">
+        <f>pbreq!V27</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI48" s="5" t="str">
+        <f>pbreq!W27</f>
+        <v>-65320.0}</v>
+      </c>
+    </row>
+    <row r="49" spans="76:87" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BX49" s="5" t="str">
+        <f>pbreq!L28</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY49" s="5" t="str">
+        <f>pbreq!M28</f>
+        <v>'rc'</v>
+      </c>
+      <c r="BZ49" s="5" t="str">
+        <f>pbreq!N28</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA49" s="5" t="str">
+        <f>pbreq!O28</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="CB49" s="5" t="str">
+        <f>pbreq!P28</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC49" s="5" t="str">
+        <f>pbreq!Q28</f>
+        <v>'Margin2'</v>
+      </c>
+      <c r="CD49" s="5" t="str">
+        <f>pbreq!R28</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE49" s="5" t="str">
+        <f>pbreq!S28</f>
+        <v>'NZD'</v>
+      </c>
+      <c r="CF49" s="5" t="str">
+        <f>pbreq!T28</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG49" s="5">
+        <f>pbreq!U28</f>
+        <v>407597</v>
+      </c>
+      <c r="CH49" s="5" t="str">
+        <f>pbreq!V28</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI49" s="5" t="str">
+        <f>pbreq!W28</f>
+        <v>-1854000.0}</v>
+      </c>
+    </row>
+    <row r="50" spans="76:87" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BX50" s="5" t="str">
+        <f>pbreq!L29</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY50" s="5" t="str">
+        <f>pbreq!M29</f>
+        <v>'rc'</v>
+      </c>
+      <c r="BZ50" s="5" t="str">
+        <f>pbreq!N29</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA50" s="5" t="str">
+        <f>pbreq!O29</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="CB50" s="5" t="str">
+        <f>pbreq!P29</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC50" s="5" t="str">
+        <f>pbreq!Q29</f>
+        <v>'Margin2'</v>
+      </c>
+      <c r="CD50" s="5" t="str">
+        <f>pbreq!R29</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE50" s="5" t="str">
+        <f>pbreq!S29</f>
+        <v>'USD'</v>
+      </c>
+      <c r="CF50" s="5" t="str">
+        <f>pbreq!T29</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG50" s="5">
+        <f>pbreq!U29</f>
+        <v>0</v>
+      </c>
+      <c r="CH50" s="5" t="str">
+        <f>pbreq!V29</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI50" s="5" t="str">
+        <f>pbreq!W29</f>
+        <v>0.0}</v>
+      </c>
+    </row>
+    <row r="51" spans="76:87" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BX51" s="5" t="str">
+        <f>pbreq!L30</f>
+        <v>{'identifier'</v>
+      </c>
+      <c r="BY51" s="5" t="str">
+        <f>pbreq!M30</f>
+        <v>'rc'</v>
+      </c>
+      <c r="BZ51" s="5" t="str">
+        <f>pbreq!N30</f>
+        <v>'bp'</v>
+      </c>
+      <c r="CA51" s="5" t="str">
+        <f>pbreq!O30</f>
+        <v>'OMF'</v>
+      </c>
+      <c r="CB51" s="5" t="str">
+        <f>pbreq!P30</f>
+        <v>'acc'</v>
+      </c>
+      <c r="CC51" s="5" t="str">
+        <f>pbreq!Q30</f>
+        <v>'Margin3'</v>
+      </c>
+      <c r="CD51" s="5" t="str">
+        <f>pbreq!R30</f>
+        <v>'curr'</v>
+      </c>
+      <c r="CE51" s="5" t="str">
+        <f>pbreq!S30</f>
+        <v>'NZD'</v>
+      </c>
+      <c r="CF51" s="5" t="str">
+        <f>pbreq!T30</f>
+        <v>'span'</v>
+      </c>
+      <c r="CG51" s="5">
+        <f>pbreq!U30</f>
+        <v>1305280</v>
+      </c>
+      <c r="CH51" s="5" t="str">
+        <f>pbreq!V30</f>
+        <v>'lfvsfv'</v>
+      </c>
+      <c r="CI51" s="5" t="str">
+        <f>pbreq!W30</f>
+        <v>-741600.0}</v>
+      </c>
+    </row>
+    <row r="52" spans="76:87" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12402,8 +15666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18:W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
complete rc, stress loss, margin, delta net exposure per account
</commit_message>
<xml_diff>
--- a/list and data.xlsx
+++ b/list and data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13320"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13320" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pa2" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3641" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3946" uniqueCount="461">
   <si>
     <t>instrument</t>
   </si>
@@ -1314,37 +1314,103 @@
     <t>final</t>
   </si>
   <si>
-    <t>'OMFRule'</t>
-  </si>
-  <si>
-    <t>'Rule'</t>
-  </si>
-  <si>
-    <t>'OMFFinal'</t>
-  </si>
-  <si>
-    <t>'Final'</t>
-  </si>
-  <si>
-    <t>'FCSRule'</t>
-  </si>
-  <si>
-    <t>'FCSFinal'</t>
-  </si>
-  <si>
     <t>'stresslconv'</t>
   </si>
   <si>
-    <t>'OMFA00000'}</t>
-  </si>
-  <si>
-    <t>'FCSU00000'}</t>
-  </si>
-  <si>
     <t xml:space="preserve">WMP   WMP       OOFC201812              201812  </t>
   </si>
   <si>
     <t>4.1.2 new price scan range rate $ = revised instrument list + price list + rc scan range csv</t>
+  </si>
+  <si>
+    <t>'BPSMargin2'</t>
+  </si>
+  <si>
+    <t>'ADMMargin1'</t>
+  </si>
+  <si>
+    <t>'BPSSum'</t>
+  </si>
+  <si>
+    <t>'ADMSum'</t>
+  </si>
+  <si>
+    <t>'FCSMargin3'</t>
+  </si>
+  <si>
+    <t>'BPSMargin4'</t>
+  </si>
+  <si>
+    <t>'FCSMargin1'</t>
+  </si>
+  <si>
+    <t>'BPSMargin3'</t>
+  </si>
+  <si>
+    <t>'ADMMargin2'</t>
+  </si>
+  <si>
+    <t>'BPSMargin6'</t>
+  </si>
+  <si>
+    <t>163635.0}</t>
+  </si>
+  <si>
+    <t>9664560.241279999}</t>
+  </si>
+  <si>
+    <t>44405.88288}</t>
+  </si>
+  <si>
+    <t>1391225.0}</t>
+  </si>
+  <si>
+    <t>3318074.92928}</t>
+  </si>
+  <si>
+    <t>81682.0}</t>
+  </si>
+  <si>
+    <t>895707.9991039999}</t>
+  </si>
+  <si>
+    <t>1746885.0}</t>
+  </si>
+  <si>
+    <t>10513905.145087998}</t>
+  </si>
+  <si>
+    <t>350640.0}</t>
+  </si>
+  <si>
+    <t>118886.92198399999}</t>
+  </si>
+  <si>
+    <t>6283.0}</t>
+  </si>
+  <si>
+    <t>447614.76863999997}</t>
+  </si>
+  <si>
+    <t>4784706.415744}</t>
+  </si>
+  <si>
+    <t>'House'</t>
+  </si>
+  <si>
+    <t>3221077.2743679998}</t>
+  </si>
+  <si>
+    <t>25513.1456}</t>
+  </si>
+  <si>
+    <t>2567939.0}</t>
+  </si>
+  <si>
+    <t>10578965.834624}</t>
+  </si>
+  <si>
+    <t>2793820.9840639997}</t>
   </si>
 </sst>
 </file>
@@ -1397,7 +1463,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1414,12 +1480,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1427,6 +1502,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Linked Cell" xfId="1" builtinId="24"/>
@@ -3511,7 +3587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CC86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD11" sqref="AD11"/>
     </sheetView>
   </sheetViews>
@@ -4981,7 +5057,7 @@
         <v>3</v>
       </c>
       <c r="AF35" s="4" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="AQ35" s="3" t="s">
         <v>116</v>
@@ -8009,7 +8085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A56" sqref="A56:F61"/>
     </sheetView>
   </sheetViews>
@@ -10790,10 +10866,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EM52"/>
+  <dimension ref="A1:EK57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AO47" sqref="AO47"/>
+    <sheetView tabSelected="1" topLeftCell="DL23" workbookViewId="0">
+      <selection activeCell="DX41" sqref="DX41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10809,9 +10885,34 @@
     <col min="27" max="27" width="7.140625" customWidth="1"/>
     <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="90" max="90" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="122" max="123" width="8" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="8" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="8" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="18" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="12" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="139" max="139" width="12" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="141" max="141" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>292</v>
       </c>
@@ -10819,7 +10920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -10848,7 +10949,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="3" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -10882,7 +10983,7 @@
       <c r="AB3" s="3"/>
       <c r="AC3" s="3"/>
     </row>
-    <row r="4" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -10917,7 +11018,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="5" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>293</v>
       </c>
@@ -10952,7 +11053,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="6" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>293</v>
       </c>
@@ -10987,7 +11088,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="7" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>310</v>
       </c>
@@ -11015,16 +11116,16 @@
       <c r="AI7" t="s">
         <v>351</v>
       </c>
-      <c r="BX7" s="3" t="str">
+      <c r="BU7" s="3" t="str">
         <f>cons!A56</f>
         <v>house</v>
       </c>
-      <c r="BY7" s="3" t="str">
+      <c r="BV7" s="3" t="str">
         <f>cons!B56</f>
         <v>list</v>
       </c>
     </row>
-    <row r="8" spans="1:81" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>293</v>
       </c>
@@ -11049,32 +11150,32 @@
       <c r="R8" t="s">
         <v>344</v>
       </c>
-      <c r="BX8" s="5" t="str">
+      <c r="BU8" s="5" t="str">
         <f>cons!A57</f>
         <v>{'bp'</v>
       </c>
-      <c r="BY8" s="5" t="str">
+      <c r="BV8" s="5" t="str">
         <f>cons!B57</f>
         <v>'ADM'</v>
       </c>
-      <c r="BZ8" s="5" t="str">
+      <c r="BW8" s="5" t="str">
         <f>cons!C57</f>
         <v>'bpid'</v>
       </c>
-      <c r="CA8" s="5" t="str">
+      <c r="BX8" s="5" t="str">
         <f>cons!D57</f>
         <v>'ADMU00000'</v>
       </c>
-      <c r="CB8" s="5" t="str">
+      <c r="BY8" s="5" t="str">
         <f>cons!E57</f>
         <v>'acc'</v>
       </c>
-      <c r="CC8" s="5" t="str">
+      <c r="BZ8" s="5" t="str">
         <f>cons!F57</f>
         <v>'Margin1'}</v>
       </c>
     </row>
-    <row r="9" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:78" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>293</v>
       </c>
@@ -11099,32 +11200,32 @@
       <c r="R9" t="s">
         <v>346</v>
       </c>
-      <c r="BX9" s="5" t="str">
+      <c r="BU9" s="5" t="str">
         <f>cons!A58</f>
         <v>{'bp'</v>
       </c>
-      <c r="BY9" s="5" t="str">
+      <c r="BV9" s="5" t="str">
         <f>cons!B58</f>
         <v>'BPS'</v>
       </c>
-      <c r="BZ9" s="5" t="str">
+      <c r="BW9" s="5" t="str">
         <f>cons!C58</f>
         <v>'bpid'</v>
       </c>
-      <c r="CA9" s="5" t="str">
+      <c r="BX9" s="5" t="str">
         <f>cons!D58</f>
         <v>'BPSS00000'</v>
       </c>
-      <c r="CB9" s="5" t="str">
+      <c r="BY9" s="5" t="str">
         <f>cons!E58</f>
         <v>'acc'</v>
       </c>
-      <c r="CC9" s="5" t="str">
+      <c r="BZ9" s="5" t="str">
         <f>cons!F58</f>
         <v>'Margin1'}</v>
       </c>
     </row>
-    <row r="10" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:78" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>293</v>
       </c>
@@ -11149,32 +11250,32 @@
       <c r="R10" t="s">
         <v>348</v>
       </c>
-      <c r="BX10" s="5" t="str">
+      <c r="BU10" s="5" t="str">
         <f>cons!A59</f>
         <v>{'bp'</v>
       </c>
-      <c r="BY10" s="5" t="str">
+      <c r="BV10" s="5" t="str">
         <f>cons!B59</f>
         <v>'FCS'</v>
       </c>
-      <c r="BZ10" s="5" t="str">
+      <c r="BW10" s="5" t="str">
         <f>cons!C59</f>
         <v>'bpid'</v>
       </c>
-      <c r="CA10" s="5" t="str">
+      <c r="BX10" s="5" t="str">
         <f>cons!D59</f>
         <v>'FCSU00000'</v>
       </c>
-      <c r="CB10" s="5" t="str">
+      <c r="BY10" s="5" t="str">
         <f>cons!E59</f>
         <v>'acc'</v>
       </c>
-      <c r="CC10" s="5" t="str">
+      <c r="BZ10" s="5" t="str">
         <f>cons!F59</f>
         <v>'Margin1'}</v>
       </c>
     </row>
-    <row r="11" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:78" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>293</v>
       </c>
@@ -11199,32 +11300,32 @@
       <c r="R11" t="s">
         <v>350</v>
       </c>
-      <c r="BX11" s="5" t="str">
+      <c r="BU11" s="5" t="str">
         <f>cons!A60</f>
         <v>{'bp'</v>
       </c>
-      <c r="BY11" s="5" t="str">
+      <c r="BV11" s="5" t="str">
         <f>cons!B60</f>
         <v>'OMF'</v>
       </c>
-      <c r="BZ11" s="5" t="str">
+      <c r="BW11" s="5" t="str">
         <f>cons!C60</f>
         <v>'bpid'</v>
       </c>
-      <c r="CA11" s="5" t="str">
+      <c r="BX11" s="5" t="str">
         <f>cons!D60</f>
         <v>'OMFA00000'</v>
       </c>
-      <c r="CB11" s="5" t="str">
+      <c r="BY11" s="5" t="str">
         <f>cons!E60</f>
         <v>'acc'</v>
       </c>
-      <c r="CC11" s="5" t="str">
+      <c r="BZ11" s="5" t="str">
         <f>cons!F60</f>
         <v>'Margin1'}</v>
       </c>
     </row>
-    <row r="12" spans="1:81" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:78" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>293</v>
       </c>
@@ -11246,32 +11347,32 @@
       <c r="G12" t="s">
         <v>311</v>
       </c>
-      <c r="BX12" s="5" t="str">
+      <c r="BU12" s="5" t="str">
         <f>cons!A61</f>
         <v>{'bp'</v>
       </c>
-      <c r="BY12" s="5" t="str">
+      <c r="BV12" s="5" t="str">
         <f>cons!B61</f>
         <v>'SFL'</v>
       </c>
-      <c r="BZ12" s="5" t="str">
+      <c r="BW12" s="5" t="str">
         <f>cons!C61</f>
         <v>'bpid'</v>
       </c>
-      <c r="CA12" s="5" t="str">
+      <c r="BX12" s="5" t="str">
         <f>cons!D61</f>
         <v>'SFLU00000'</v>
       </c>
-      <c r="CB12" s="5" t="str">
+      <c r="BY12" s="5" t="str">
         <f>cons!E61</f>
         <v>'acc'</v>
       </c>
-      <c r="CC12" s="5" t="str">
+      <c r="BZ12" s="5" t="str">
         <f>cons!F61</f>
         <v>'Margin1'}</v>
       </c>
     </row>
-    <row r="13" spans="1:81" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>310</v>
       </c>
@@ -11300,7 +11401,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>315</v>
       </c>
@@ -11314,7 +11415,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>315</v>
       </c>
@@ -11328,7 +11429,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="16" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>315</v>
       </c>
@@ -11342,7 +11443,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="17" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>315</v>
       </c>
@@ -11360,7 +11461,7 @@
         <v>currency</v>
       </c>
     </row>
-    <row r="18" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:141" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>315</v>
       </c>
@@ -11398,7 +11499,7 @@
         <v>1.481701}</v>
       </c>
     </row>
-    <row r="19" spans="1:143" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:141" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>315</v>
       </c>
@@ -11412,7 +11513,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="20" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>315</v>
       </c>
@@ -11420,7 +11521,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="21" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>315</v>
       </c>
@@ -11443,7 +11544,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>315</v>
       </c>
@@ -11469,7 +11570,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="23" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>315</v>
       </c>
@@ -11495,7 +11596,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="24" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U24" t="s">
         <v>315</v>
       </c>
@@ -11579,7 +11680,7 @@
       </c>
       <c r="DS24" s="3"/>
     </row>
-    <row r="25" spans="1:143" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U25" t="s">
         <v>315</v>
       </c>
@@ -11688,92 +11789,47 @@
       <c r="DJ25" t="s">
         <v>419</v>
       </c>
-      <c r="DL25" t="s">
+      <c r="DM25" t="s">
         <v>315</v>
       </c>
-      <c r="DM25" t="s">
-        <v>340</v>
-      </c>
-      <c r="DN25" t="s">
+      <c r="DO25" t="s">
         <v>26</v>
       </c>
-      <c r="DO25" t="s">
-        <v>367</v>
-      </c>
-      <c r="DP25" t="s">
+      <c r="DQ25" t="s">
         <v>378</v>
       </c>
-      <c r="DQ25">
-        <v>0</v>
-      </c>
-      <c r="DR25" t="s">
+      <c r="DS25" t="s">
+        <v>385</v>
+      </c>
+      <c r="DU25" t="s">
+        <v>412</v>
+      </c>
+      <c r="DW25" t="s">
         <v>394</v>
       </c>
-      <c r="DS25">
-        <v>0</v>
-      </c>
-      <c r="DT25" t="s">
-        <v>412</v>
-      </c>
-      <c r="DU25">
-        <v>0</v>
-      </c>
-      <c r="DV25" t="s">
-        <v>385</v>
-      </c>
-      <c r="DW25">
-        <v>0</v>
-      </c>
-      <c r="DX25" t="s">
+      <c r="DY25" t="s">
         <v>413</v>
       </c>
-      <c r="DY25" t="s">
-        <v>420</v>
-      </c>
-      <c r="DZ25" t="s">
+      <c r="EA25" t="s">
         <v>414</v>
       </c>
-      <c r="EA25">
-        <v>0</v>
-      </c>
-      <c r="EB25" t="s">
+      <c r="EC25" t="s">
         <v>399</v>
       </c>
-      <c r="EC25">
-        <v>0</v>
-      </c>
-      <c r="ED25" t="s">
+      <c r="EE25" t="s">
         <v>415</v>
       </c>
-      <c r="EE25">
-        <v>0</v>
-      </c>
-      <c r="EF25" t="s">
+      <c r="EG25" t="s">
         <v>416</v>
       </c>
-      <c r="EG25">
-        <v>0</v>
-      </c>
-      <c r="EH25" t="s">
+      <c r="EI25" t="s">
         <v>417</v>
       </c>
-      <c r="EI25">
-        <v>0</v>
-      </c>
-      <c r="EJ25" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK25">
-        <v>0</v>
-      </c>
-      <c r="EL25" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM25" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="26" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="EK25" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="26" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U26" t="s">
         <v>315</v>
       </c>
@@ -11886,7 +11942,7 @@
         <v>315</v>
       </c>
       <c r="DM26" t="s">
-        <v>340</v>
+        <v>432</v>
       </c>
       <c r="DN26" t="s">
         <v>26</v>
@@ -11901,34 +11957,34 @@
         <v>0</v>
       </c>
       <c r="DR26" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS26">
-        <v>-741600</v>
+        <v>0</v>
       </c>
       <c r="DT26" t="s">
         <v>412</v>
       </c>
       <c r="DU26">
-        <v>1305280</v>
+        <v>0</v>
       </c>
       <c r="DV26" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW26">
-        <v>1305280</v>
+        <v>0</v>
       </c>
       <c r="DX26" t="s">
         <v>413</v>
       </c>
       <c r="DY26" t="s">
-        <v>420</v>
+        <v>455</v>
       </c>
       <c r="DZ26" t="s">
         <v>414</v>
       </c>
       <c r="EA26">
-        <v>-741600</v>
+        <v>0</v>
       </c>
       <c r="EB26" t="s">
         <v>399</v>
@@ -11940,7 +11996,7 @@
         <v>415</v>
       </c>
       <c r="EE26">
-        <v>-741600</v>
+        <v>0</v>
       </c>
       <c r="EF26" t="s">
         <v>416</v>
@@ -11952,24 +12008,18 @@
         <v>417</v>
       </c>
       <c r="EI26">
-        <v>1305280</v>
+        <v>0</v>
       </c>
       <c r="EJ26" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK26">
-        <v>1305280</v>
-      </c>
-      <c r="EL26" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM26" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="27" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:141" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="U27" t="s">
         <v>315</v>
@@ -12083,7 +12133,7 @@
         <v>315</v>
       </c>
       <c r="DM27" t="s">
-        <v>337</v>
+        <v>432</v>
       </c>
       <c r="DN27" t="s">
         <v>26</v>
@@ -12095,10 +12145,10 @@
         <v>378</v>
       </c>
       <c r="DQ27">
-        <v>6705.9059999999999</v>
+        <v>0</v>
       </c>
       <c r="DR27" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS27">
         <v>0</v>
@@ -12107,25 +12157,25 @@
         <v>412</v>
       </c>
       <c r="DU27">
-        <v>2662.5</v>
+        <v>0</v>
       </c>
       <c r="DV27" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW27">
-        <v>17077.5</v>
+        <v>0</v>
       </c>
       <c r="DX27" t="s">
         <v>413</v>
       </c>
       <c r="DY27" t="s">
-        <v>352</v>
+        <v>455</v>
       </c>
       <c r="DZ27" t="s">
         <v>414</v>
       </c>
       <c r="EA27">
-        <v>6705.9059999999999</v>
+        <v>0</v>
       </c>
       <c r="EB27" t="s">
         <v>399</v>
@@ -12137,7 +12187,7 @@
         <v>415</v>
       </c>
       <c r="EE27">
-        <v>9936.1476261059997</v>
+        <v>0</v>
       </c>
       <c r="EF27" t="s">
         <v>416</v>
@@ -12149,22 +12199,16 @@
         <v>417</v>
       </c>
       <c r="EI27">
-        <v>25303.7488275</v>
+        <v>0</v>
       </c>
       <c r="EJ27" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK27">
-        <v>3945.0289124999999</v>
-      </c>
-      <c r="EL27" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM27" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="28" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:141" x14ac:dyDescent="0.25">
       <c r="F28">
         <f>LEN(F27)</f>
         <v>48</v>
@@ -12281,7 +12325,7 @@
         <v>315</v>
       </c>
       <c r="DM28" t="s">
-        <v>337</v>
+        <v>439</v>
       </c>
       <c r="DN28" t="s">
         <v>26</v>
@@ -12296,73 +12340,67 @@
         <v>0</v>
       </c>
       <c r="DR28" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS28">
-        <v>0</v>
+        <v>37440</v>
       </c>
       <c r="DT28" t="s">
         <v>412</v>
       </c>
       <c r="DU28">
-        <v>0</v>
+        <v>81682</v>
       </c>
       <c r="DV28" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW28">
-        <v>0</v>
+        <v>945360</v>
       </c>
       <c r="DX28" t="s">
         <v>413</v>
       </c>
       <c r="DY28" t="s">
-        <v>352</v>
+        <v>420</v>
       </c>
       <c r="DZ28" t="s">
         <v>414</v>
       </c>
       <c r="EA28">
-        <v>0</v>
+        <v>945360</v>
       </c>
       <c r="EB28" t="s">
         <v>399</v>
       </c>
       <c r="EC28">
-        <v>0</v>
+        <v>44242</v>
       </c>
       <c r="ED28" t="s">
         <v>415</v>
       </c>
       <c r="EE28">
-        <v>0</v>
+        <v>945360</v>
       </c>
       <c r="EF28" t="s">
         <v>416</v>
       </c>
       <c r="EG28">
-        <v>0</v>
+        <v>44242</v>
       </c>
       <c r="EH28" t="s">
         <v>417</v>
       </c>
       <c r="EI28">
-        <v>0</v>
+        <v>37440</v>
       </c>
       <c r="EJ28" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK28">
-        <v>0</v>
-      </c>
-      <c r="EL28" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM28" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="29" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK28" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="29" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U29" t="s">
         <v>315</v>
       </c>
@@ -12475,7 +12513,7 @@
         <v>315</v>
       </c>
       <c r="DM29" t="s">
-        <v>341</v>
+        <v>439</v>
       </c>
       <c r="DN29" t="s">
         <v>26</v>
@@ -12487,76 +12525,70 @@
         <v>378</v>
       </c>
       <c r="DQ29">
-        <v>1948.175</v>
+        <v>0</v>
       </c>
       <c r="DR29" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS29">
-        <v>0</v>
+        <v>708723</v>
       </c>
       <c r="DT29" t="s">
         <v>412</v>
       </c>
       <c r="DU29">
-        <v>0</v>
+        <v>2295445</v>
       </c>
       <c r="DV29" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW29">
-        <v>0</v>
+        <v>-10445300</v>
       </c>
       <c r="DX29" t="s">
         <v>413</v>
       </c>
       <c r="DY29" t="s">
-        <v>352</v>
+        <v>420</v>
       </c>
       <c r="DZ29" t="s">
         <v>414</v>
       </c>
       <c r="EA29">
-        <v>1948.175</v>
+        <v>-10445300</v>
       </c>
       <c r="EB29" t="s">
         <v>399</v>
       </c>
       <c r="EC29">
-        <v>0</v>
+        <v>1586722</v>
       </c>
       <c r="ED29" t="s">
         <v>415</v>
       </c>
       <c r="EE29">
-        <v>2886.6128456749998</v>
+        <v>-15098722.9312</v>
       </c>
       <c r="EF29" t="s">
         <v>416</v>
       </c>
       <c r="EG29">
-        <v>0</v>
+        <v>2293612.99788799</v>
       </c>
       <c r="EH29" t="s">
         <v>417</v>
       </c>
       <c r="EI29">
-        <v>0</v>
+        <v>1024461.93139199</v>
       </c>
       <c r="EJ29" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK29">
-        <v>0</v>
-      </c>
-      <c r="EL29" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM29" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="30" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK29" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U30" t="s">
         <v>315</v>
       </c>
@@ -12669,7 +12701,7 @@
         <v>315</v>
       </c>
       <c r="DM30" t="s">
-        <v>341</v>
+        <v>434</v>
       </c>
       <c r="DN30" t="s">
         <v>26</v>
@@ -12684,22 +12716,22 @@
         <v>0</v>
       </c>
       <c r="DR30" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS30">
-        <v>0</v>
+        <v>37440</v>
       </c>
       <c r="DT30" t="s">
         <v>412</v>
       </c>
       <c r="DU30">
-        <v>0</v>
+        <v>81682</v>
       </c>
       <c r="DV30" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW30">
-        <v>0</v>
+        <v>945360</v>
       </c>
       <c r="DX30" t="s">
         <v>413</v>
@@ -12711,46 +12743,40 @@
         <v>414</v>
       </c>
       <c r="EA30">
-        <v>0</v>
+        <v>945360</v>
       </c>
       <c r="EB30" t="s">
         <v>399</v>
       </c>
       <c r="EC30">
-        <v>0</v>
+        <v>44242</v>
       </c>
       <c r="ED30" t="s">
         <v>415</v>
       </c>
       <c r="EE30">
-        <v>0</v>
+        <v>945360</v>
       </c>
       <c r="EF30" t="s">
         <v>416</v>
       </c>
       <c r="EG30">
-        <v>0</v>
+        <v>44242</v>
       </c>
       <c r="EH30" t="s">
         <v>417</v>
       </c>
       <c r="EI30">
-        <v>0</v>
+        <v>37440</v>
       </c>
       <c r="EJ30" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK30">
-        <v>0</v>
-      </c>
-      <c r="EL30" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM30" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="31" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK30" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="31" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U31" t="s">
         <v>315</v>
       </c>
@@ -12862,62 +12888,83 @@
       <c r="DL31" t="s">
         <v>315</v>
       </c>
-      <c r="DM31" t="s">
-        <v>338</v>
-      </c>
-      <c r="DN31" t="s">
+      <c r="DM31" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="DN31" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="DO31" t="s">
+      <c r="DO31" s="7" t="s">
         <v>367</v>
       </c>
-      <c r="DP31" t="s">
+      <c r="DP31" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="DQ31">
+      <c r="DQ31" s="7">
         <v>0</v>
       </c>
-      <c r="DR31" t="s">
+      <c r="DR31" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS31" s="7">
+        <v>708723</v>
+      </c>
+      <c r="DT31" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU31" s="7">
+        <v>2295445</v>
+      </c>
+      <c r="DV31" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="DS31">
-        <v>-65320</v>
-      </c>
-      <c r="DT31" t="s">
-        <v>412</v>
-      </c>
-      <c r="DU31">
-        <v>16330</v>
-      </c>
-      <c r="DV31" t="s">
-        <v>385</v>
-      </c>
-      <c r="DW31">
-        <v>16330</v>
-      </c>
-      <c r="DX31" t="s">
+      <c r="DW31" s="7">
+        <v>-10445300</v>
+      </c>
+      <c r="DX31" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="DY31" t="s">
-        <v>420</v>
-      </c>
-      <c r="DZ31" t="s">
+      <c r="DY31" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ31" s="7" t="s">
         <v>414</v>
       </c>
-      <c r="EA31">
-        <v>-65320</v>
-      </c>
-      <c r="EB31" t="s">
+      <c r="EA31" s="7">
+        <v>-10445300</v>
+      </c>
+      <c r="EB31" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="EC31">
-        <v>0</v>
-      </c>
-      <c r="ED31" t="s">
+      <c r="EC31" s="7">
+        <v>1586722</v>
+      </c>
+      <c r="ED31" s="7" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="32" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="EE31" s="7">
+        <v>-15098722.9312</v>
+      </c>
+      <c r="EF31" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG31" s="7">
+        <v>2293612.99788799</v>
+      </c>
+      <c r="EH31" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI31" s="7">
+        <v>1024461.93139199</v>
+      </c>
+      <c r="EJ31" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK31" s="7" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="32" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U32" t="s">
         <v>315</v>
       </c>
@@ -13026,35 +13073,86 @@
       <c r="DJ32" t="s">
         <v>392</v>
       </c>
-      <c r="DL32">
-        <v>-96784.709319999994</v>
+      <c r="DL32" t="s">
+        <v>315</v>
       </c>
       <c r="DM32" t="s">
+        <v>431</v>
+      </c>
+      <c r="DN32" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO32" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP32" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ32">
+        <v>0</v>
+      </c>
+      <c r="DR32" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS32">
+        <v>0</v>
+      </c>
+      <c r="DT32" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU32">
+        <v>0</v>
+      </c>
+      <c r="DV32" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW32">
+        <v>0</v>
+      </c>
+      <c r="DX32" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY32" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ32" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA32">
+        <v>0</v>
+      </c>
+      <c r="EB32" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC32">
+        <v>0</v>
+      </c>
+      <c r="ED32" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE32">
+        <v>0</v>
+      </c>
+      <c r="EF32" t="s">
         <v>416</v>
       </c>
-      <c r="DN32">
+      <c r="EG32">
         <v>0</v>
       </c>
-      <c r="DO32" t="s">
+      <c r="EH32" t="s">
         <v>417</v>
       </c>
-      <c r="DP32">
-        <v>24196.177329999999</v>
-      </c>
-      <c r="DQ32" t="s">
-        <v>434</v>
-      </c>
-      <c r="DR32">
-        <v>24196.177329999999</v>
-      </c>
-      <c r="DS32" t="s">
-        <v>403</v>
-      </c>
-      <c r="DT32" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="33" spans="1:143" x14ac:dyDescent="0.25">
+      <c r="EI32">
+        <v>0</v>
+      </c>
+      <c r="EJ32" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:141" x14ac:dyDescent="0.25">
       <c r="U33" t="s">
         <v>315</v>
       </c>
@@ -13167,37 +13265,37 @@
         <v>315</v>
       </c>
       <c r="DM33" t="s">
-        <v>338</v>
+        <v>431</v>
       </c>
       <c r="DN33" t="s">
         <v>26</v>
       </c>
       <c r="DO33" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="DP33" t="s">
         <v>378</v>
       </c>
       <c r="DQ33">
-        <v>0</v>
+        <v>646074.30000000005</v>
       </c>
       <c r="DR33" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS33">
-        <v>0</v>
+        <v>974710</v>
       </c>
       <c r="DT33" t="s">
         <v>412</v>
       </c>
       <c r="DU33">
-        <v>0</v>
+        <v>3310061</v>
       </c>
       <c r="DV33" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW33">
-        <v>0</v>
+        <v>14862740</v>
       </c>
       <c r="DX33" t="s">
         <v>413</v>
@@ -13209,46 +13307,40 @@
         <v>414</v>
       </c>
       <c r="EA33">
-        <v>0</v>
+        <v>15508814.300000001</v>
       </c>
       <c r="EB33" t="s">
         <v>399</v>
       </c>
       <c r="EC33">
-        <v>0</v>
+        <v>2335351</v>
       </c>
       <c r="ED33" t="s">
         <v>415</v>
       </c>
       <c r="EE33">
-        <v>0</v>
+        <v>22418053.105907101</v>
       </c>
       <c r="EF33" t="s">
         <v>416</v>
       </c>
       <c r="EG33">
-        <v>0</v>
+        <v>3375759.2119039898</v>
       </c>
       <c r="EH33" t="s">
         <v>417</v>
       </c>
       <c r="EI33">
-        <v>0</v>
+        <v>1408947.2038399901</v>
       </c>
       <c r="EJ33" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK33">
-        <v>0</v>
-      </c>
-      <c r="EL33" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM33" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="34" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK33" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="34" spans="1:141" x14ac:dyDescent="0.25">
       <c r="AA34" s="3" t="s">
         <v>1</v>
       </c>
@@ -13364,37 +13456,37 @@
         <v>315</v>
       </c>
       <c r="DM34" t="s">
-        <v>336</v>
+        <v>438</v>
       </c>
       <c r="DN34" t="s">
         <v>26</v>
       </c>
       <c r="DO34" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="DP34" t="s">
         <v>378</v>
       </c>
       <c r="DQ34">
-        <v>1948.175</v>
+        <v>0</v>
       </c>
       <c r="DR34" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS34">
-        <v>0</v>
+        <v>2880</v>
       </c>
       <c r="DT34" t="s">
         <v>412</v>
       </c>
       <c r="DU34">
-        <v>0</v>
+        <v>6283</v>
       </c>
       <c r="DV34" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW34">
-        <v>0</v>
+        <v>72720</v>
       </c>
       <c r="DX34" t="s">
         <v>413</v>
@@ -13406,46 +13498,40 @@
         <v>414</v>
       </c>
       <c r="EA34">
-        <v>1948.175</v>
+        <v>72720</v>
       </c>
       <c r="EB34" t="s">
         <v>399</v>
       </c>
       <c r="EC34">
-        <v>0</v>
+        <v>3403</v>
       </c>
       <c r="ED34" t="s">
         <v>415</v>
       </c>
       <c r="EE34">
-        <v>2886.6128456749998</v>
+        <v>72720</v>
       </c>
       <c r="EF34" t="s">
         <v>416</v>
       </c>
       <c r="EG34">
-        <v>0</v>
+        <v>3403</v>
       </c>
       <c r="EH34" t="s">
         <v>417</v>
       </c>
       <c r="EI34">
-        <v>0</v>
+        <v>2880</v>
       </c>
       <c r="EJ34" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK34">
-        <v>0</v>
-      </c>
-      <c r="EL34" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM34" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="35" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK34" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="35" spans="1:141" x14ac:dyDescent="0.25">
       <c r="AA35" t="s">
         <v>323</v>
       </c>
@@ -13594,13 +13680,13 @@
         <v>315</v>
       </c>
       <c r="DM35" t="s">
-        <v>336</v>
+        <v>438</v>
       </c>
       <c r="DN35" t="s">
         <v>26</v>
       </c>
       <c r="DO35" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="DP35" t="s">
         <v>378</v>
@@ -13609,22 +13695,22 @@
         <v>0</v>
       </c>
       <c r="DR35" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS35">
-        <v>-1854000</v>
+        <v>22320</v>
       </c>
       <c r="DT35" t="s">
         <v>412</v>
       </c>
       <c r="DU35">
-        <v>407597</v>
+        <v>82246</v>
       </c>
       <c r="DV35" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW35">
-        <v>407597</v>
+        <v>-368700</v>
       </c>
       <c r="DX35" t="s">
         <v>413</v>
@@ -13636,46 +13722,40 @@
         <v>414</v>
       </c>
       <c r="EA35">
-        <v>-1854000</v>
+        <v>-368700</v>
       </c>
       <c r="EB35" t="s">
         <v>399</v>
       </c>
       <c r="EC35">
-        <v>0</v>
+        <v>59926</v>
       </c>
       <c r="ED35" t="s">
         <v>415</v>
       </c>
       <c r="EE35">
-        <v>-1854000</v>
+        <v>-532957.32479999994</v>
       </c>
       <c r="EF35" t="s">
         <v>416</v>
       </c>
       <c r="EG35">
-        <v>0</v>
+        <v>86623.272703999901</v>
       </c>
       <c r="EH35" t="s">
         <v>417</v>
       </c>
       <c r="EI35">
-        <v>407597</v>
+        <v>32263.6492799999</v>
       </c>
       <c r="EJ35" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK35">
-        <v>407597</v>
-      </c>
-      <c r="EL35" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM35" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="36" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK35" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="36" spans="1:141" x14ac:dyDescent="0.25">
       <c r="AA36" t="s">
         <v>323</v>
       </c>
@@ -13824,37 +13904,37 @@
         <v>315</v>
       </c>
       <c r="DM36" t="s">
-        <v>339</v>
+        <v>436</v>
       </c>
       <c r="DN36" t="s">
         <v>26</v>
       </c>
       <c r="DO36" t="s">
-        <v>367</v>
+        <v>380</v>
       </c>
       <c r="DP36" t="s">
         <v>378</v>
       </c>
       <c r="DQ36">
-        <v>6705.9059999999999</v>
+        <v>0</v>
       </c>
       <c r="DR36" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS36">
-        <v>0</v>
+        <v>786000</v>
       </c>
       <c r="DT36" t="s">
         <v>412</v>
       </c>
       <c r="DU36">
-        <v>2662.5</v>
+        <v>1746885</v>
       </c>
       <c r="DV36" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW36">
-        <v>2662.5</v>
+        <v>-14671800</v>
       </c>
       <c r="DX36" t="s">
         <v>413</v>
@@ -13866,46 +13946,40 @@
         <v>414</v>
       </c>
       <c r="EA36">
-        <v>6705.9059999999999</v>
+        <v>-14671800</v>
       </c>
       <c r="EB36" t="s">
         <v>399</v>
       </c>
       <c r="EC36">
-        <v>0</v>
+        <v>960885</v>
       </c>
       <c r="ED36" t="s">
         <v>415</v>
       </c>
       <c r="EE36">
-        <v>9936.1476261059997</v>
+        <v>-14671800</v>
       </c>
       <c r="EF36" t="s">
         <v>416</v>
       </c>
       <c r="EG36">
-        <v>0</v>
+        <v>960885</v>
       </c>
       <c r="EH36" t="s">
         <v>417</v>
       </c>
       <c r="EI36">
-        <v>3945.0289124999999</v>
+        <v>786000</v>
       </c>
       <c r="EJ36" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK36">
-        <v>3945.0289124999999</v>
-      </c>
-      <c r="EL36" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM36" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="37" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK36" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="37" spans="1:141" x14ac:dyDescent="0.25">
       <c r="AA37" t="s">
         <v>323</v>
       </c>
@@ -13958,37 +14032,37 @@
         <v>315</v>
       </c>
       <c r="DM37" t="s">
-        <v>339</v>
+        <v>436</v>
       </c>
       <c r="DN37" t="s">
         <v>26</v>
       </c>
       <c r="DO37" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="DP37" t="s">
         <v>378</v>
       </c>
       <c r="DQ37">
-        <v>0</v>
+        <v>15.809999999999899</v>
       </c>
       <c r="DR37" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="DS37">
-        <v>0</v>
+        <v>175116</v>
       </c>
       <c r="DT37" t="s">
         <v>412</v>
       </c>
       <c r="DU37">
-        <v>0</v>
+        <v>619651</v>
       </c>
       <c r="DV37" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="DW37">
-        <v>0</v>
+        <v>-2634875</v>
       </c>
       <c r="DX37" t="s">
         <v>413</v>
@@ -14000,46 +14074,40 @@
         <v>414</v>
       </c>
       <c r="EA37">
-        <v>0</v>
+        <v>-2634859.19</v>
       </c>
       <c r="EB37" t="s">
         <v>399</v>
       </c>
       <c r="EC37">
-        <v>0</v>
+        <v>444535</v>
       </c>
       <c r="ED37" t="s">
         <v>415</v>
       </c>
       <c r="EE37">
-        <v>0</v>
+        <v>-3808699.4985817499</v>
       </c>
       <c r="EF37" t="s">
         <v>416</v>
       </c>
       <c r="EG37">
-        <v>0</v>
+        <v>642577.12063999998</v>
       </c>
       <c r="EH37" t="s">
         <v>417</v>
       </c>
       <c r="EI37">
-        <v>0</v>
+        <v>253130.87846399899</v>
       </c>
       <c r="EJ37" t="s">
-        <v>434</v>
-      </c>
-      <c r="EK37">
-        <v>0</v>
-      </c>
-      <c r="EL37" t="s">
-        <v>403</v>
-      </c>
-      <c r="EM37" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="38" spans="1:143" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+      <c r="EK37" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="38" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>1</v>
       </c>
@@ -14101,7 +14169,7 @@
         <v>315</v>
       </c>
       <c r="DM38" t="s">
-        <v>428</v>
+        <v>440</v>
       </c>
       <c r="DN38" t="s">
         <v>26</v>
@@ -14110,25 +14178,73 @@
         <v>380</v>
       </c>
       <c r="DP38" t="s">
-        <v>413</v>
-      </c>
-      <c r="DQ38" t="s">
-        <v>429</v>
+        <v>378</v>
+      </c>
+      <c r="DQ38">
+        <v>0</v>
       </c>
       <c r="DR38" t="s">
-        <v>416</v>
+        <v>385</v>
       </c>
       <c r="DS38">
         <v>0</v>
       </c>
       <c r="DT38" t="s">
-        <v>403</v>
-      </c>
-      <c r="DU38" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="39" spans="1:143" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+      <c r="DU38">
+        <v>0</v>
+      </c>
+      <c r="DV38" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW38">
+        <v>0</v>
+      </c>
+      <c r="DX38" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY38" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ38" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA38">
+        <v>0</v>
+      </c>
+      <c r="EB38" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC38">
+        <v>0</v>
+      </c>
+      <c r="ED38" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE38">
+        <v>0</v>
+      </c>
+      <c r="EF38" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG38">
+        <v>0</v>
+      </c>
+      <c r="EH38" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI38">
+        <v>0</v>
+      </c>
+      <c r="EJ38" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK38" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:141" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>323</v>
       </c>
@@ -14189,34 +14305,82 @@
         <v>315</v>
       </c>
       <c r="DM39" t="s">
-        <v>430</v>
+        <v>440</v>
       </c>
       <c r="DN39" t="s">
         <v>26</v>
       </c>
       <c r="DO39" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="DP39" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ39">
+        <v>0</v>
+      </c>
+      <c r="DR39" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS39">
+        <v>95700</v>
+      </c>
+      <c r="DT39" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU39">
+        <v>309660</v>
+      </c>
+      <c r="DV39" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW39">
+        <v>-1548300</v>
+      </c>
+      <c r="DX39" t="s">
         <v>413</v>
       </c>
-      <c r="DQ39" t="s">
-        <v>431</v>
-      </c>
-      <c r="DR39" t="s">
+      <c r="DY39" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ39" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA39">
+        <v>-1548300</v>
+      </c>
+      <c r="EB39" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC39">
+        <v>213960</v>
+      </c>
+      <c r="ED39" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE39">
+        <v>-2238073.8432</v>
+      </c>
+      <c r="EF39" t="s">
         <v>416</v>
       </c>
-      <c r="DS39">
-        <v>0</v>
-      </c>
-      <c r="DT39" t="s">
-        <v>403</v>
-      </c>
-      <c r="DU39" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="40" spans="1:143" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="EG39">
+        <v>309280.03583999898</v>
+      </c>
+      <c r="EH39" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI39">
+        <v>138334.7328</v>
+      </c>
+      <c r="EJ39" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK39" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:141" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>323</v>
       </c>
@@ -14317,7 +14481,7 @@
         <v>315</v>
       </c>
       <c r="DM40" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="DN40" t="s">
         <v>26</v>
@@ -14326,25 +14490,73 @@
         <v>380</v>
       </c>
       <c r="DP40" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ40">
+        <v>0</v>
+      </c>
+      <c r="DR40" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS40">
+        <v>625920</v>
+      </c>
+      <c r="DT40" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU40">
+        <v>1391225</v>
+      </c>
+      <c r="DV40" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW40">
+        <v>-14599080</v>
+      </c>
+      <c r="DX40" t="s">
         <v>413</v>
       </c>
-      <c r="DQ40" t="s">
-        <v>429</v>
-      </c>
-      <c r="DR40" t="s">
+      <c r="DY40" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ40" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA40">
+        <v>-14599080</v>
+      </c>
+      <c r="EB40" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC40">
+        <v>765305</v>
+      </c>
+      <c r="ED40" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE40">
+        <v>-14599080</v>
+      </c>
+      <c r="EF40" t="s">
         <v>416</v>
       </c>
-      <c r="DS40">
-        <v>0</v>
-      </c>
-      <c r="DT40" t="s">
-        <v>403</v>
-      </c>
-      <c r="DU40" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="41" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="EG40">
+        <v>765305</v>
+      </c>
+      <c r="EH40" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI40">
+        <v>625920</v>
+      </c>
+      <c r="EJ40" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK40" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="41" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BX41" s="5" t="str">
         <f>pbreq!L20</f>
         <v>{'identifier'</v>
@@ -14393,38 +14605,86 @@
         <f>pbreq!W20</f>
         <v>0.0}</v>
       </c>
-      <c r="DL41" t="s">
+      <c r="DL41" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="DM41" t="s">
+      <c r="DM41" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="DN41" t="s">
+      <c r="DN41" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="DO41" t="s">
-        <v>380</v>
-      </c>
-      <c r="DP41" t="s">
+      <c r="DO41" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP41" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ41" s="7">
+        <v>646090.11</v>
+      </c>
+      <c r="DR41" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS41" s="7">
+        <v>582645</v>
+      </c>
+      <c r="DT41" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU41" s="7">
+        <v>1932766</v>
+      </c>
+      <c r="DV41" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW41" s="7">
+        <v>10310865</v>
+      </c>
+      <c r="DX41" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="DQ41" t="s">
-        <v>431</v>
-      </c>
-      <c r="DR41" t="s">
+      <c r="DY41" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ41" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA41" s="7">
+        <v>10956955.109999999</v>
+      </c>
+      <c r="EB41" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC41" s="7">
+        <v>1350121</v>
+      </c>
+      <c r="ED41" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE41" s="7">
+        <v>15838322.4393254</v>
+      </c>
+      <c r="EF41" s="7" t="s">
         <v>416</v>
       </c>
-      <c r="DS41">
-        <v>0</v>
-      </c>
-      <c r="DT41" t="s">
-        <v>403</v>
-      </c>
-      <c r="DU41" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="42" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="EG41" s="7">
+        <v>1951605.305984</v>
+      </c>
+      <c r="EH41" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI41" s="7">
+        <v>842215.67807999998</v>
+      </c>
+      <c r="EJ41" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK41" s="7" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="42" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AR42" s="3" t="s">
         <v>1</v>
       </c>
@@ -14494,8 +14754,86 @@
         <f>pbreq!W21</f>
         <v>0.0}</v>
       </c>
-    </row>
-    <row r="43" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL42" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM42" t="s">
+        <v>437</v>
+      </c>
+      <c r="DN42" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO42" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP42" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ42">
+        <v>0</v>
+      </c>
+      <c r="DR42" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS42">
+        <v>0</v>
+      </c>
+      <c r="DT42" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU42">
+        <v>0</v>
+      </c>
+      <c r="DV42" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW42">
+        <v>0</v>
+      </c>
+      <c r="DX42" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY42" t="s">
+        <v>455</v>
+      </c>
+      <c r="DZ42" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA42">
+        <v>0</v>
+      </c>
+      <c r="EB42" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC42">
+        <v>0</v>
+      </c>
+      <c r="ED42" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE42">
+        <v>0</v>
+      </c>
+      <c r="EF42" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG42">
+        <v>0</v>
+      </c>
+      <c r="EH42" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI42">
+        <v>0</v>
+      </c>
+      <c r="EJ42" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AR43" t="s">
         <v>323</v>
       </c>
@@ -14616,8 +14954,86 @@
         <f>pbreq!W22</f>
         <v>-1854000.0}</v>
       </c>
-    </row>
-    <row r="44" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL43" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM43" t="s">
+        <v>437</v>
+      </c>
+      <c r="DN43" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO43" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP43" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ43">
+        <v>0</v>
+      </c>
+      <c r="DR43" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS43">
+        <v>707385</v>
+      </c>
+      <c r="DT43" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU43">
+        <v>2228342</v>
+      </c>
+      <c r="DV43" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW43">
+        <v>10676610</v>
+      </c>
+      <c r="DX43" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY43" t="s">
+        <v>455</v>
+      </c>
+      <c r="DZ43" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA43">
+        <v>10676610</v>
+      </c>
+      <c r="EB43" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC43">
+        <v>1520957</v>
+      </c>
+      <c r="ED43" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE43">
+        <v>15433082.4614399</v>
+      </c>
+      <c r="EF43" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG43">
+        <v>2198549.4273279998</v>
+      </c>
+      <c r="EH43" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI43">
+        <v>1022527.84703999</v>
+      </c>
+      <c r="EJ43" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK43" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="44" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O44" s="5" t="str">
         <f>'pa2'!N82</f>
         <v>option</v>
@@ -14818,8 +15234,86 @@
         <f>pbreq!W23</f>
         <v>0.0}</v>
       </c>
-    </row>
-    <row r="45" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL44" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM44" t="s">
+        <v>338</v>
+      </c>
+      <c r="DN44" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO44" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP44" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ44">
+        <v>0</v>
+      </c>
+      <c r="DR44" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS44">
+        <v>0</v>
+      </c>
+      <c r="DT44" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU44">
+        <v>0</v>
+      </c>
+      <c r="DV44" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW44">
+        <v>0</v>
+      </c>
+      <c r="DX44" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY44" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ44" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA44">
+        <v>0</v>
+      </c>
+      <c r="EB44" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC44">
+        <v>0</v>
+      </c>
+      <c r="ED44" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE44">
+        <v>0</v>
+      </c>
+      <c r="EF44" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG44">
+        <v>0</v>
+      </c>
+      <c r="EH44" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI44">
+        <v>0</v>
+      </c>
+      <c r="EJ44" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK44" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O45" t="str">
         <f>'pa2'!N83</f>
         <v>{'comm'</v>
@@ -15052,8 +15546,86 @@
         <f>pbreq!W24</f>
         <v>-741600.0}</v>
       </c>
-    </row>
-    <row r="46" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL45" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM45" t="s">
+        <v>338</v>
+      </c>
+      <c r="DN45" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO45" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP45" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ45">
+        <v>4208498.16</v>
+      </c>
+      <c r="DR45" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS45">
+        <v>1990689</v>
+      </c>
+      <c r="DT45" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU45">
+        <v>6685945</v>
+      </c>
+      <c r="DV45" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW45">
+        <v>16038390</v>
+      </c>
+      <c r="DX45" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY45" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ45" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA45">
+        <v>20246888.16</v>
+      </c>
+      <c r="EB45" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC45">
+        <v>4695256</v>
+      </c>
+      <c r="ED45" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE45">
+        <v>29266957.822832599</v>
+      </c>
+      <c r="EF45" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG45">
+        <v>6787011.3290239898</v>
+      </c>
+      <c r="EH45" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI45">
+        <v>2877548.9122559899</v>
+      </c>
+      <c r="EJ45" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK45" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="46" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O46" t="str">
         <f>'pa2'!N84</f>
         <v>{'comm'</v>
@@ -15286,8 +15858,86 @@
         <f>pbreq!W25</f>
         <v>-65320.0}</v>
       </c>
-    </row>
-    <row r="47" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL46" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM46" t="s">
+        <v>435</v>
+      </c>
+      <c r="DN46" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO46" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP46" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ46">
+        <v>0</v>
+      </c>
+      <c r="DR46" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS46">
+        <v>0</v>
+      </c>
+      <c r="DT46" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU46">
+        <v>0</v>
+      </c>
+      <c r="DV46" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW46">
+        <v>0</v>
+      </c>
+      <c r="DX46" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY46" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ46" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA46">
+        <v>0</v>
+      </c>
+      <c r="EB46" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC46">
+        <v>0</v>
+      </c>
+      <c r="ED46" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE46">
+        <v>0</v>
+      </c>
+      <c r="EF46" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG46">
+        <v>0</v>
+      </c>
+      <c r="EH46" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI46">
+        <v>0</v>
+      </c>
+      <c r="EJ46" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O47" t="str">
         <f>'pa2'!N85</f>
         <v>{'comm'</v>
@@ -15448,8 +16098,86 @@
         <f>pbreq!W26</f>
         <v>0.0}</v>
       </c>
-    </row>
-    <row r="48" spans="1:143" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL47" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM47" t="s">
+        <v>435</v>
+      </c>
+      <c r="DN47" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO47" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP47" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ47">
+        <v>0</v>
+      </c>
+      <c r="DR47" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS47">
+        <v>10800</v>
+      </c>
+      <c r="DT47" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU47">
+        <v>30720</v>
+      </c>
+      <c r="DV47" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW47">
+        <v>-153600</v>
+      </c>
+      <c r="DX47" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY47" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ47" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA47">
+        <v>-153600</v>
+      </c>
+      <c r="EB47" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC47">
+        <v>19920</v>
+      </c>
+      <c r="ED47" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE47">
+        <v>-222029.41439999899</v>
+      </c>
+      <c r="EF47" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG47">
+        <v>28794.439679999999</v>
+      </c>
+      <c r="EH47" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI47">
+        <v>15611.4432</v>
+      </c>
+      <c r="EJ47" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK47" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="48" spans="1:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="O48" t="str">
         <f>'pa2'!N86</f>
         <v>{'comm'</v>
@@ -15610,8 +16338,86 @@
         <f>pbreq!W27</f>
         <v>-65320.0}</v>
       </c>
-    </row>
-    <row r="49" spans="76:87" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL48" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM48" t="s">
+        <v>339</v>
+      </c>
+      <c r="DN48" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO48" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP48" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ48">
+        <v>1737826.2</v>
+      </c>
+      <c r="DR48" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS48">
+        <v>1252600</v>
+      </c>
+      <c r="DT48" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU48">
+        <v>2567939</v>
+      </c>
+      <c r="DV48" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW48">
+        <v>17089920</v>
+      </c>
+      <c r="DX48" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY48" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ48" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA48">
+        <v>18827746.199999999</v>
+      </c>
+      <c r="EB48" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC48">
+        <v>1315339</v>
+      </c>
+      <c r="ED48" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE48">
+        <v>18827746.199999999</v>
+      </c>
+      <c r="EF48" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG48">
+        <v>1315339</v>
+      </c>
+      <c r="EH48" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI48">
+        <v>1252600</v>
+      </c>
+      <c r="EJ48" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK48" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="49" spans="76:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BX49" s="5" t="str">
         <f>pbreq!L28</f>
         <v>{'identifier'</v>
@@ -15660,8 +16466,86 @@
         <f>pbreq!W28</f>
         <v>-1854000.0}</v>
       </c>
-    </row>
-    <row r="50" spans="76:87" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL49" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM49" t="s">
+        <v>339</v>
+      </c>
+      <c r="DN49" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO49" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP49" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ49">
+        <v>0</v>
+      </c>
+      <c r="DR49" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS49">
+        <v>4875</v>
+      </c>
+      <c r="DT49" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU49">
+        <v>17650</v>
+      </c>
+      <c r="DV49" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW49">
+        <v>70625</v>
+      </c>
+      <c r="DX49" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY49" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ49" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA49">
+        <v>70625</v>
+      </c>
+      <c r="EB49" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC49">
+        <v>12775</v>
+      </c>
+      <c r="ED49" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE49">
+        <v>102088.719999999</v>
+      </c>
+      <c r="EF49" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG49">
+        <v>18466.313599999899</v>
+      </c>
+      <c r="EH49" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI49">
+        <v>7046.8319999999903</v>
+      </c>
+      <c r="EJ49" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK49" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="50" spans="76:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BX50" s="5" t="str">
         <f>pbreq!L29</f>
         <v>{'identifier'</v>
@@ -15710,8 +16594,86 @@
         <f>pbreq!W29</f>
         <v>0.0}</v>
       </c>
-    </row>
-    <row r="51" spans="76:87" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="DL50" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM50" t="s">
+        <v>337</v>
+      </c>
+      <c r="DN50" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO50" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP50" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ50">
+        <v>1737826.2</v>
+      </c>
+      <c r="DR50" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS50">
+        <v>1252600</v>
+      </c>
+      <c r="DT50" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU50">
+        <v>2567939</v>
+      </c>
+      <c r="DV50" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW50">
+        <v>17089920</v>
+      </c>
+      <c r="DX50" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY50" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ50" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA50">
+        <v>18827746.199999999</v>
+      </c>
+      <c r="EB50" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC50">
+        <v>1315339</v>
+      </c>
+      <c r="ED50" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE50">
+        <v>18827746.199999999</v>
+      </c>
+      <c r="EF50" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG50">
+        <v>1315339</v>
+      </c>
+      <c r="EH50" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI50">
+        <v>1252600</v>
+      </c>
+      <c r="EJ50" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK50" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="51" spans="76:141" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="BX51" s="5" t="str">
         <f>pbreq!L30</f>
         <v>{'identifier'</v>
@@ -15760,9 +16722,570 @@
         <f>pbreq!W30</f>
         <v>-741600.0}</v>
       </c>
-    </row>
-    <row r="52" spans="76:87" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="DL51" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM51" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="DN51" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO51" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP51" s="7" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ51" s="7">
+        <v>4208498.16</v>
+      </c>
+      <c r="DR51" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS51" s="7">
+        <v>2176953</v>
+      </c>
+      <c r="DT51" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU51" s="7">
+        <v>7318531</v>
+      </c>
+      <c r="DV51" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW51" s="7">
+        <v>26632025</v>
+      </c>
+      <c r="DX51" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY51" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ51" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA51" s="7">
+        <v>30840523.16</v>
+      </c>
+      <c r="EB51" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC51" s="7">
+        <v>5141578</v>
+      </c>
+      <c r="ED51" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE51" s="7">
+        <v>44580099.589872599</v>
+      </c>
+      <c r="EF51" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG51" s="7">
+        <v>7432171.5653119897</v>
+      </c>
+      <c r="EH51" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI51" s="7">
+        <v>3146794.2693119999</v>
+      </c>
+      <c r="EJ51" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK51" s="7" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="52" spans="76:141" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="DL52" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM52" t="s">
+        <v>336</v>
+      </c>
+      <c r="DN52" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO52" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP52" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ52">
+        <v>-1737826.2</v>
+      </c>
+      <c r="DR52" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS52">
+        <v>63000</v>
+      </c>
+      <c r="DT52" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU52">
+        <v>350640</v>
+      </c>
+      <c r="DV52" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW52">
+        <v>-2534400</v>
+      </c>
+      <c r="DX52" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY52" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ52" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA52">
+        <v>-4272226.2</v>
+      </c>
+      <c r="EB52" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC52">
+        <v>287640</v>
+      </c>
+      <c r="ED52" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE52">
+        <v>-4272226.2</v>
+      </c>
+      <c r="EF52" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG52">
+        <v>287640</v>
+      </c>
+      <c r="EH52" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI52">
+        <v>63000</v>
+      </c>
+      <c r="EJ52" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK52" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="53" spans="76:141" x14ac:dyDescent="0.25">
+      <c r="DL53" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM53" t="s">
+        <v>336</v>
+      </c>
+      <c r="DN53" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO53" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP53" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ53">
+        <v>-4854588.2699999996</v>
+      </c>
+      <c r="DR53" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS53">
+        <v>2209645</v>
+      </c>
+      <c r="DT53" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU53">
+        <v>7273522</v>
+      </c>
+      <c r="DV53" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW53">
+        <v>-26497590</v>
+      </c>
+      <c r="DX53" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY53" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ53" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA53">
+        <v>-31352178.27</v>
+      </c>
+      <c r="EB53" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC53">
+        <v>5063877</v>
+      </c>
+      <c r="ED53" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE53">
+        <v>-45319699.097998001</v>
+      </c>
+      <c r="EF53" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG53">
+        <v>7319854.4590079999</v>
+      </c>
+      <c r="EH53" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI53">
+        <v>3194050.6860799999</v>
+      </c>
+      <c r="EJ53" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK53" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="54" spans="76:141" x14ac:dyDescent="0.25">
+      <c r="DL54" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM54" t="s">
+        <v>340</v>
+      </c>
+      <c r="DN54" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO54" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP54" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ54">
+        <v>0</v>
+      </c>
+      <c r="DR54" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS54">
+        <v>6823725</v>
+      </c>
+      <c r="DT54" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU54">
+        <v>163635</v>
+      </c>
+      <c r="DV54" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW54">
+        <v>-901800</v>
+      </c>
+      <c r="DX54" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY54" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ54" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA54">
+        <v>-901800</v>
+      </c>
+      <c r="EB54" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC54">
+        <v>0</v>
+      </c>
+      <c r="ED54" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE54">
+        <v>-901800</v>
+      </c>
+      <c r="EF54" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG54">
+        <v>0</v>
+      </c>
+      <c r="EH54" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI54">
+        <v>6823725</v>
+      </c>
+      <c r="EJ54" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK54" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="55" spans="76:141" x14ac:dyDescent="0.25">
+      <c r="DL55" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM55" t="s">
+        <v>340</v>
+      </c>
+      <c r="DN55" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO55" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP55" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ55">
+        <v>0</v>
+      </c>
+      <c r="DR55" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS55">
+        <v>0</v>
+      </c>
+      <c r="DT55" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU55">
+        <v>0</v>
+      </c>
+      <c r="DV55" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW55">
+        <v>0</v>
+      </c>
+      <c r="DX55" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY55" t="s">
+        <v>420</v>
+      </c>
+      <c r="DZ55" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA55">
+        <v>0</v>
+      </c>
+      <c r="EB55" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC55">
+        <v>0</v>
+      </c>
+      <c r="ED55" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE55">
+        <v>0</v>
+      </c>
+      <c r="EF55" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG55">
+        <v>0</v>
+      </c>
+      <c r="EH55" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI55">
+        <v>0</v>
+      </c>
+      <c r="EJ55" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK55" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="76:141" x14ac:dyDescent="0.25">
+      <c r="DL56" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM56" t="s">
+        <v>341</v>
+      </c>
+      <c r="DN56" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO56" t="s">
+        <v>380</v>
+      </c>
+      <c r="DP56" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ56">
+        <v>-1737826.2</v>
+      </c>
+      <c r="DR56" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS56">
+        <v>63000</v>
+      </c>
+      <c r="DT56" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU56">
+        <v>350640</v>
+      </c>
+      <c r="DV56" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW56">
+        <v>-2534400</v>
+      </c>
+      <c r="DX56" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY56" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ56" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA56">
+        <v>-4272226.2</v>
+      </c>
+      <c r="EB56" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC56">
+        <v>287640</v>
+      </c>
+      <c r="ED56" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE56">
+        <v>-4272226.2</v>
+      </c>
+      <c r="EF56" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG56">
+        <v>287640</v>
+      </c>
+      <c r="EH56" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI56">
+        <v>63000</v>
+      </c>
+      <c r="EJ56" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK56" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="57" spans="76:141" x14ac:dyDescent="0.25">
+      <c r="DL57" t="s">
+        <v>315</v>
+      </c>
+      <c r="DM57" t="s">
+        <v>341</v>
+      </c>
+      <c r="DN57" t="s">
+        <v>26</v>
+      </c>
+      <c r="DO57" t="s">
+        <v>367</v>
+      </c>
+      <c r="DP57" t="s">
+        <v>378</v>
+      </c>
+      <c r="DQ57">
+        <v>-4854588.2699999996</v>
+      </c>
+      <c r="DR57" t="s">
+        <v>385</v>
+      </c>
+      <c r="DS57">
+        <v>2209645</v>
+      </c>
+      <c r="DT57" t="s">
+        <v>412</v>
+      </c>
+      <c r="DU57">
+        <v>7273522</v>
+      </c>
+      <c r="DV57" t="s">
+        <v>394</v>
+      </c>
+      <c r="DW57">
+        <v>-26497590</v>
+      </c>
+      <c r="DX57" t="s">
+        <v>413</v>
+      </c>
+      <c r="DY57" t="s">
+        <v>352</v>
+      </c>
+      <c r="DZ57" t="s">
+        <v>414</v>
+      </c>
+      <c r="EA57">
+        <v>-31352178.27</v>
+      </c>
+      <c r="EB57" t="s">
+        <v>399</v>
+      </c>
+      <c r="EC57">
+        <v>5063877</v>
+      </c>
+      <c r="ED57" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE57">
+        <v>-45319699.097998001</v>
+      </c>
+      <c r="EF57" t="s">
+        <v>416</v>
+      </c>
+      <c r="EG57">
+        <v>7319854.4590079999</v>
+      </c>
+      <c r="EH57" t="s">
+        <v>417</v>
+      </c>
+      <c r="EI57">
+        <v>3194050.6860799999</v>
+      </c>
+      <c r="EJ57" t="s">
+        <v>428</v>
+      </c>
+      <c r="EK57" t="s">
+        <v>449</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="DL26:EK57">
+    <sortCondition ref="DM26:DM57"/>
+    <sortCondition ref="DO26:DO57"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -15773,7 +17296,7 @@
   <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="L19" sqref="L19:W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>